<commit_message>
Fixes #357 Documentation instead of _Documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW-Dev\2R\Excel_Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0518B4-3DE8-4ACB-BBF5-34D575A784AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="863" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="863" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="_readme" sheetId="8" r:id="rId1"/>
-    <sheet name="_Documentation" sheetId="12" r:id="rId2"/>
+    <sheet name="Documentation" sheetId="12" r:id="rId2"/>
     <sheet name="Workflow and Tasks" sheetId="13" r:id="rId3"/>
     <sheet name="SimulationSets" sheetId="20" r:id="rId4"/>
     <sheet name="Outputs_1" sheetId="5" r:id="rId5"/>
@@ -42,12 +41,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Katrin Coboeken</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -203,12 +202,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Katrin Coboeken</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -283,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000004000000}">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -312,12 +311,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Katrin Coboeken</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -342,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -366,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000003000000}">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000004000000}">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1928,7 +1927,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2133,18 +2132,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2160,7 +2159,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2235,23 +2234,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2287,23 +2269,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2479,23 +2444,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="128.8984375" customWidth="1"/>
+    <col min="1" max="1" width="3.375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="128.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>113</v>
       </c>
@@ -2503,7 +2468,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>114</v>
       </c>
@@ -2511,7 +2476,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -2519,7 +2484,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -2527,7 +2492,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2535,7 +2500,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -2550,17 +2515,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B262A-9A5B-46FC-A725-85413523FCCF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -2568,13 +2533,13 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2587,29 +2552,29 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>359</v>
       </c>
@@ -2621,20 +2586,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>360</v>
       </c>
@@ -2657,7 +2622,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>70</v>
       </c>
@@ -2672,7 +2637,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>73</v>
       </c>
@@ -2687,7 +2652,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>75</v>
       </c>
@@ -2704,7 +2669,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>78</v>
       </c>
@@ -2721,7 +2686,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>81</v>
       </c>
@@ -2738,7 +2703,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>83</v>
       </c>
@@ -2753,7 +2718,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>85</v>
       </c>
@@ -2774,7 +2739,7 @@
       </c>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>91</v>
       </c>
@@ -2795,7 +2760,7 @@
       </c>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>96</v>
       </c>
@@ -2816,7 +2781,7 @@
       </c>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>101</v>
       </c>
@@ -2837,7 +2802,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>105</v>
       </c>
@@ -2866,30 +2831,30 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -2903,7 +2868,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50</v>
       </c>
@@ -2918,7 +2883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>A4+10</f>
         <v>60</v>
@@ -2936,7 +2901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ref="A6:B10" si="1">A5+10</f>
         <v>70</v>
@@ -2954,7 +2919,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2972,7 +2937,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -2990,7 +2955,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3008,7 +2973,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -3034,30 +2999,30 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -3071,7 +3036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>50</v>
       </c>
@@ -3086,7 +3051,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>A4+10</f>
         <v>60</v>
@@ -3104,7 +3069,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ref="A6:B10" si="1">A5+10</f>
         <v>70</v>
@@ -3122,7 +3087,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -3140,7 +3105,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -3158,7 +3123,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3176,7 +3141,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -3202,7 +3167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39160AF7-ED4A-459F-ABF7-9A3E8B4E93E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3210,21 +3175,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>128</v>
       </c>
@@ -3259,7 +3224,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3294,7 +3259,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -3329,7 +3294,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>133</v>
       </c>
@@ -3349,7 +3314,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>189</v>
       </c>
@@ -3366,7 +3331,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>190</v>
       </c>
@@ -3380,7 +3345,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>191</v>
       </c>
@@ -3394,7 +3359,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>192</v>
       </c>
@@ -3408,7 +3373,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>193</v>
       </c>
@@ -3422,7 +3387,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>194</v>
       </c>
@@ -3433,7 +3398,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>195</v>
       </c>
@@ -3444,7 +3409,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>196</v>
       </c>
@@ -3455,7 +3420,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>197</v>
       </c>
@@ -3466,7 +3431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>198</v>
       </c>
@@ -3477,7 +3442,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>199</v>
       </c>
@@ -3488,7 +3453,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>200</v>
       </c>
@@ -3499,7 +3464,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>201</v>
       </c>
@@ -3510,7 +3475,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>202</v>
       </c>
@@ -3521,7 +3486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>203</v>
       </c>
@@ -3532,7 +3497,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>204</v>
       </c>
@@ -3543,7 +3508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>205</v>
       </c>
@@ -3554,7 +3519,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>206</v>
       </c>
@@ -3565,7 +3530,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>207</v>
       </c>
@@ -3573,7 +3538,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>208</v>
       </c>
@@ -3581,7 +3546,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
         <v>209</v>
       </c>
@@ -3589,7 +3554,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>210</v>
       </c>
@@ -3597,7 +3562,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>211</v>
       </c>
@@ -3605,7 +3570,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>212</v>
       </c>
@@ -3613,7 +3578,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>213</v>
       </c>
@@ -3621,42 +3586,42 @@
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>261</v>
       </c>
@@ -3668,19 +3633,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.09765625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>117</v>
       </c>
@@ -3688,7 +3653,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>118</v>
       </c>
@@ -3696,7 +3661,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>119</v>
       </c>
@@ -3711,7 +3676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFA2222-53E9-4EC9-97BD-22D97A0BEE05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3719,15 +3684,15 @@
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.19921875" customWidth="1"/>
-    <col min="3" max="3" width="36.69921875" customWidth="1"/>
-    <col min="6" max="6" width="22.69921875" customWidth="1"/>
+    <col min="2" max="2" width="100.25" customWidth="1"/>
+    <col min="3" max="3" width="36.75" customWidth="1"/>
+    <col min="6" max="6" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3738,7 +3703,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>125</v>
       </c>
@@ -3746,7 +3711,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>126</v>
       </c>
@@ -3757,7 +3722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>155</v>
       </c>
@@ -3768,7 +3733,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>157</v>
       </c>
@@ -3779,7 +3744,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>362</v>
       </c>
@@ -3787,11 +3752,11 @@
         <v>363</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>137</v>
       </c>
@@ -3802,7 +3767,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>139</v>
       </c>
@@ -3813,7 +3778,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>141</v>
       </c>
@@ -3824,7 +3789,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>143</v>
       </c>
@@ -3835,7 +3800,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>145</v>
       </c>
@@ -3846,7 +3811,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>147</v>
       </c>
@@ -3857,7 +3822,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>149</v>
       </c>
@@ -3868,7 +3833,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>150</v>
       </c>
@@ -3879,7 +3844,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>151</v>
       </c>
@@ -3890,11 +3855,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>159</v>
       </c>
@@ -3902,7 +3867,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>160</v>
       </c>
@@ -3913,7 +3878,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>164</v>
       </c>
@@ -3921,7 +3886,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>165</v>
       </c>
@@ -3929,7 +3894,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>167</v>
       </c>
@@ -3940,7 +3905,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>168</v>
       </c>
@@ -3948,7 +3913,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>182</v>
       </c>
@@ -3956,7 +3921,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>174</v>
       </c>
@@ -3964,7 +3929,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>175</v>
       </c>
@@ -3972,7 +3937,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>178</v>
       </c>
@@ -3980,7 +3945,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>180</v>
       </c>
@@ -3994,25 +3959,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4DD5E394-DB56-4CF9-8843-782939E4B76D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41782F69-4DE6-4E69-99A4-8E5A162A7617}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C9B617F-76A5-4A18-8C52-8FC6FCDC5553}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{27F5C9CF-E08E-451A-BDCC-8583F3505D62}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
@@ -4025,23 +3990,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BE365A-43FF-4890-B212-B66C20B6B64E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.8984375" customWidth="1"/>
-    <col min="2" max="2" width="42.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.796875" customWidth="1"/>
-    <col min="4" max="4" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="42.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -4055,7 +4020,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>321</v>
       </c>
@@ -4069,7 +4034,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>327</v>
       </c>
@@ -4077,7 +4042,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>328</v>
       </c>
@@ -4085,7 +4050,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -4099,7 +4064,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>332</v>
       </c>
@@ -4107,7 +4072,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>339</v>
       </c>
@@ -4121,7 +4086,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>335</v>
       </c>
@@ -4135,7 +4100,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="69" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>313</v>
       </c>
@@ -4149,21 +4114,21 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>370</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="29" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>343</v>
       </c>
@@ -4177,7 +4142,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>364</v>
       </c>
@@ -4191,15 +4156,15 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
         <v>345</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>346</v>
       </c>
@@ -4207,7 +4172,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>348</v>
       </c>
@@ -4215,7 +4180,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>350</v>
       </c>
@@ -4229,7 +4194,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>369</v>
       </c>
@@ -4241,7 +4206,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>352</v>
       </c>
@@ -4255,7 +4220,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>353</v>
       </c>
@@ -4269,23 +4234,23 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
     </row>
@@ -4298,19 +4263,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5EFC9B10-DECD-48CD-8E33-903B2F25A5CD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>C7:D7 C18:D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{11FC722F-66CC-4E80-9F92-2FC30700F6DD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C11:D12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EF3833C-AEDC-4515-860C-DDCECEDDAE3A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
@@ -4323,7 +4288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4331,16 +4296,16 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="47.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.19921875" customWidth="1"/>
+    <col min="1" max="1" width="15.75" style="10" customWidth="1"/>
+    <col min="2" max="2" width="30.625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4357,7 +4322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>310</v>
       </c>
@@ -4372,7 +4337,7 @@
       </c>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>312</v>
       </c>
@@ -4386,7 +4351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -4400,7 +4365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="69" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>313</v>
       </c>
@@ -4411,21 +4376,21 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>373</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>317</v>
       </c>
@@ -4447,7 +4412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1C5AA6-6C28-45A7-A61F-94EA6ED12211}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4455,21 +4420,21 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.69921875" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.8984375" customWidth="1"/>
+    <col min="11" max="11" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -4506,7 +4471,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -4517,7 +4482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4534,7 +4499,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F43B6CDB-3D36-4EF0-9917-43F9D77E3707}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$J$2:$J$22</xm:f>
           </x14:formula1>
@@ -4547,7 +4512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB85399-C384-4052-AD23-5D6464C511C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4555,13 +4520,13 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -4572,7 +4537,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -4583,7 +4548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -4594,7 +4559,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -4605,7 +4570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -4616,7 +4581,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>227</v>
       </c>
@@ -4627,7 +4592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>262</v>
       </c>
@@ -4638,7 +4603,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -4649,7 +4614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -4660,7 +4625,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -4671,7 +4636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -4682,7 +4647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -4693,7 +4658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -4704,7 +4669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -4715,7 +4680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>274</v>
       </c>
@@ -4726,7 +4691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>275</v>
       </c>
@@ -4737,7 +4702,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>276</v>
       </c>
@@ -4748,7 +4713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>277</v>
       </c>
@@ -4759,7 +4724,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>278</v>
       </c>
@@ -4770,7 +4735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>279</v>
       </c>
@@ -4781,7 +4746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>280</v>
       </c>
@@ -4792,7 +4757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>281</v>
       </c>
@@ -4803,7 +4768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>282</v>
       </c>
@@ -4814,7 +4779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>283</v>
       </c>
@@ -4825,7 +4790,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>284</v>
       </c>
@@ -4836,7 +4801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>285</v>
       </c>
@@ -4847,7 +4812,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>286</v>
       </c>
@@ -4858,7 +4823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>287</v>
       </c>
@@ -4869,7 +4834,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>288</v>
       </c>
@@ -4880,7 +4845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>289</v>
       </c>
@@ -4891,7 +4856,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="20" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>290</v>
       </c>
@@ -4902,7 +4867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -4913,7 +4878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -4930,31 +4895,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7D8034F5-F038-4A88-A601-98CC4D69608C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3 C5 C15:C18 C21:C22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE3D08DE-0C99-4CD2-8223-9013CFD55000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C4 C10:C11 C19:C20 C31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7E518415-2322-41FC-855A-3FB40C3BC649}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>C6:C9 C23:C30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D16BAC09-CAEC-43D5-9320-25A8CF7CC57C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>C12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{67C41D50-AA7D-45A0-B781-0061D0D7CB6E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
@@ -4967,7 +4932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD82E6C-E443-4C43-8643-8E84848061C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4975,12 +4940,12 @@
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -4988,67 +4953,67 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -5059,31 +5024,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F59A8D5D-A393-43F4-84C9-BF447EFC7A68}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE3D8966-4A59-4DEA-A20D-9AC15BD1AFD0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C11ECD2-0203-4A95-A38B-283F848B1898}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>B6:B9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CF4AECF-E0BB-4CAE-B96C-B1762FD18C30}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B10:B11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE34ECD6-E16F-4201-A20B-33E78AF770A5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
@@ -5096,7 +5061,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8231F15-242A-43E7-9329-8D29896849C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5104,12 +5069,12 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -5117,137 +5082,137 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>290</v>
       </c>
       <c r="B23" s="20"/>
     </row>
-    <row r="24" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D8EFB88-1407-4DC4-A3DB-56CA143B999B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B3 B7:B10 B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6256903-5087-4BC2-831D-B18268CDE6CD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B5:B6 B11:B12 B23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CC30E241-3CB2-4609-ADDF-4B7243E7756F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Revert update of Excel template in inst/extdata
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW-Dev\2R\Excel_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0518B4-3DE8-4ACB-BBF5-34D575A784AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="863" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="863" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_readme" sheetId="8" r:id="rId1"/>
-    <sheet name="Documentation" sheetId="12" r:id="rId2"/>
+    <sheet name="_Documentation" sheetId="12" r:id="rId2"/>
     <sheet name="Workflow and Tasks" sheetId="13" r:id="rId3"/>
     <sheet name="SimulationSets" sheetId="20" r:id="rId4"/>
     <sheet name="Outputs_1" sheetId="5" r:id="rId5"/>
@@ -41,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Katrin Coboeken</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -202,12 +203,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Katrin Coboeken</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -232,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -256,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -282,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000004000000}">
       <text>
         <r>
           <rPr>
@@ -311,12 +312,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Katrin Coboeken</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -341,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -365,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000003000000}">
       <text>
         <r>
           <rPr>
@@ -391,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1927,7 +1928,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2132,18 +2133,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2159,7 +2160,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2234,6 +2235,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2269,6 +2287,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2444,23 +2479,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="128.875" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="128.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>113</v>
       </c>
@@ -2468,7 +2503,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>114</v>
       </c>
@@ -2476,7 +2511,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -2484,7 +2519,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -2492,7 +2527,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -2500,7 +2535,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -2515,17 +2550,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B262A-9A5B-46FC-A725-85413523FCCF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -2533,13 +2568,13 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2552,29 +2587,29 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>359</v>
       </c>
@@ -2586,20 +2621,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>360</v>
       </c>
@@ -2622,7 +2657,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>70</v>
       </c>
@@ -2637,7 +2672,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>73</v>
       </c>
@@ -2652,7 +2687,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>75</v>
       </c>
@@ -2669,7 +2704,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="69" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>78</v>
       </c>
@@ -2686,7 +2721,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>81</v>
       </c>
@@ -2703,7 +2738,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>83</v>
       </c>
@@ -2718,7 +2753,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>85</v>
       </c>
@@ -2739,7 +2774,7 @@
       </c>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>91</v>
       </c>
@@ -2760,7 +2795,7 @@
       </c>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>96</v>
       </c>
@@ -2781,7 +2816,7 @@
       </c>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>101</v>
       </c>
@@ -2802,7 +2837,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>105</v>
       </c>
@@ -2831,30 +2866,30 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -2868,7 +2903,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -2883,7 +2918,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+10</f>
         <v>60</v>
@@ -2901,7 +2936,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:B10" si="1">A5+10</f>
         <v>70</v>
@@ -2919,7 +2954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2937,7 +2972,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -2955,7 +2990,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2973,7 +3008,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -2999,30 +3034,30 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -3036,7 +3071,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -3051,7 +3086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+10</f>
         <v>60</v>
@@ -3069,7 +3104,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:B10" si="1">A5+10</f>
         <v>70</v>
@@ -3087,7 +3122,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -3105,7 +3140,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -3123,7 +3158,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3141,7 +3176,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -3167,7 +3202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39160AF7-ED4A-459F-ABF7-9A3E8B4E93E8}">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3175,21 +3210,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>128</v>
       </c>
@@ -3224,7 +3259,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3259,7 +3294,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -3294,7 +3329,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>133</v>
       </c>
@@ -3314,7 +3349,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>189</v>
       </c>
@@ -3331,7 +3366,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>190</v>
       </c>
@@ -3345,7 +3380,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>191</v>
       </c>
@@ -3359,7 +3394,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>192</v>
       </c>
@@ -3373,7 +3408,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>193</v>
       </c>
@@ -3387,7 +3422,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>194</v>
       </c>
@@ -3398,7 +3433,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>195</v>
       </c>
@@ -3409,7 +3444,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>196</v>
       </c>
@@ -3420,7 +3455,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>197</v>
       </c>
@@ -3431,7 +3466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>198</v>
       </c>
@@ -3442,7 +3477,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>199</v>
       </c>
@@ -3453,7 +3488,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>200</v>
       </c>
@@ -3464,7 +3499,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>201</v>
       </c>
@@ -3475,7 +3510,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>202</v>
       </c>
@@ -3486,7 +3521,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>203</v>
       </c>
@@ -3497,7 +3532,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>204</v>
       </c>
@@ -3508,7 +3543,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>205</v>
       </c>
@@ -3519,7 +3554,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>206</v>
       </c>
@@ -3530,7 +3565,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>207</v>
       </c>
@@ -3538,7 +3573,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>208</v>
       </c>
@@ -3546,7 +3581,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>209</v>
       </c>
@@ -3554,7 +3589,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>210</v>
       </c>
@@ -3562,7 +3597,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>211</v>
       </c>
@@ -3570,7 +3605,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>212</v>
       </c>
@@ -3578,7 +3613,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>213</v>
       </c>
@@ -3586,42 +3621,42 @@
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
         <v>261</v>
       </c>
@@ -3633,19 +3668,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>117</v>
       </c>
@@ -3653,7 +3688,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>118</v>
       </c>
@@ -3661,7 +3696,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>119</v>
       </c>
@@ -3676,7 +3711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFA2222-53E9-4EC9-97BD-22D97A0BEE05}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3684,15 +3719,15 @@
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.25" customWidth="1"/>
-    <col min="3" max="3" width="36.75" customWidth="1"/>
-    <col min="6" max="6" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="100.19921875" customWidth="1"/>
+    <col min="3" max="3" width="36.69921875" customWidth="1"/>
+    <col min="6" max="6" width="22.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3703,7 +3738,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>125</v>
       </c>
@@ -3711,7 +3746,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>126</v>
       </c>
@@ -3722,7 +3757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>155</v>
       </c>
@@ -3733,7 +3768,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>157</v>
       </c>
@@ -3744,7 +3779,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>362</v>
       </c>
@@ -3752,11 +3787,11 @@
         <v>363</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>137</v>
       </c>
@@ -3767,7 +3802,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>139</v>
       </c>
@@ -3778,7 +3813,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>141</v>
       </c>
@@ -3789,7 +3824,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>143</v>
       </c>
@@ -3800,7 +3835,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>145</v>
       </c>
@@ -3811,7 +3846,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>147</v>
       </c>
@@ -3822,7 +3857,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>149</v>
       </c>
@@ -3833,7 +3868,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>150</v>
       </c>
@@ -3844,7 +3879,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>151</v>
       </c>
@@ -3855,11 +3890,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>159</v>
       </c>
@@ -3867,7 +3902,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>160</v>
       </c>
@@ -3878,7 +3913,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>164</v>
       </c>
@@ -3886,7 +3921,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>165</v>
       </c>
@@ -3894,7 +3929,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>167</v>
       </c>
@@ -3905,7 +3940,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>168</v>
       </c>
@@ -3913,7 +3948,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>182</v>
       </c>
@@ -3921,7 +3956,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>174</v>
       </c>
@@ -3929,7 +3964,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>175</v>
       </c>
@@ -3937,7 +3972,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>178</v>
       </c>
@@ -3945,7 +3980,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>180</v>
       </c>
@@ -3959,25 +3994,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4DD5E394-DB56-4CF9-8843-782939E4B76D}">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41782F69-4DE6-4E69-99A4-8E5A162A7617}">
           <x14:formula1>
             <xm:f>Lookup!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C9B617F-76A5-4A18-8C52-8FC6FCDC5553}">
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{27F5C9CF-E08E-451A-BDCC-8583F3505D62}">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
@@ -3990,23 +4025,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BE365A-43FF-4890-B212-B66C20B6B64E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="42.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.75" customWidth="1"/>
-    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.8984375" customWidth="1"/>
+    <col min="2" max="2" width="42.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.796875" customWidth="1"/>
+    <col min="4" max="4" width="29.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -4020,7 +4055,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>321</v>
       </c>
@@ -4034,7 +4069,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>327</v>
       </c>
@@ -4042,7 +4077,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>328</v>
       </c>
@@ -4050,7 +4085,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -4064,7 +4099,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>332</v>
       </c>
@@ -4072,7 +4107,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>339</v>
       </c>
@@ -4086,7 +4121,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>335</v>
       </c>
@@ -4100,7 +4135,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="69" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>313</v>
       </c>
@@ -4114,21 +4149,21 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>371</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="30" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>343</v>
       </c>
@@ -4142,7 +4177,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>364</v>
       </c>
@@ -4156,15 +4191,15 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+    </row>
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>346</v>
       </c>
@@ -4172,7 +4207,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>348</v>
       </c>
@@ -4180,7 +4215,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>350</v>
       </c>
@@ -4194,7 +4229,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>369</v>
       </c>
@@ -4206,7 +4241,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>352</v>
       </c>
@@ -4220,7 +4255,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>353</v>
       </c>
@@ -4234,23 +4269,23 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="7"/>
     </row>
@@ -4263,19 +4298,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5EFC9B10-DECD-48CD-8E33-903B2F25A5CD}">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>C7:D7 C18:D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{11FC722F-66CC-4E80-9F92-2FC30700F6DD}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C11:D12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EF3833C-AEDC-4515-860C-DDCECEDDAE3A}">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
@@ -4288,7 +4323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4296,16 +4331,16 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" style="10" customWidth="1"/>
-    <col min="2" max="2" width="30.625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="15.69921875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="47.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4322,7 +4357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>310</v>
       </c>
@@ -4337,7 +4372,7 @@
       </c>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>312</v>
       </c>
@@ -4351,7 +4386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -4365,7 +4400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="69" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>313</v>
       </c>
@@ -4376,21 +4411,21 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="30" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>317</v>
       </c>
@@ -4412,7 +4447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1C5AA6-6C28-45A7-A61F-94EA6ED12211}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4420,21 +4455,21 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.69921875" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="22.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -4471,7 +4506,7 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -4482,7 +4517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4499,7 +4534,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F43B6CDB-3D36-4EF0-9917-43F9D77E3707}">
           <x14:formula1>
             <xm:f>Lookup!$J$2:$J$22</xm:f>
           </x14:formula1>
@@ -4512,7 +4547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB85399-C384-4052-AD23-5D6464C511C8}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4520,13 +4555,13 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -4537,7 +4572,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -4548,7 +4583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -4559,7 +4594,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -4570,7 +4605,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -4581,7 +4616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>227</v>
       </c>
@@ -4592,7 +4627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>262</v>
       </c>
@@ -4603,7 +4638,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -4614,7 +4649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -4625,7 +4660,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -4636,7 +4671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -4647,7 +4682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -4658,7 +4693,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -4669,7 +4704,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -4680,7 +4715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>274</v>
       </c>
@@ -4691,7 +4726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>275</v>
       </c>
@@ -4702,7 +4737,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>276</v>
       </c>
@@ -4713,7 +4748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>277</v>
       </c>
@@ -4724,7 +4759,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>278</v>
       </c>
@@ -4735,7 +4770,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>279</v>
       </c>
@@ -4746,7 +4781,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>280</v>
       </c>
@@ -4757,7 +4792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>281</v>
       </c>
@@ -4768,7 +4803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>282</v>
       </c>
@@ -4779,7 +4814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>283</v>
       </c>
@@ -4790,7 +4825,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>284</v>
       </c>
@@ -4801,7 +4836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>285</v>
       </c>
@@ -4812,7 +4847,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>286</v>
       </c>
@@ -4823,7 +4858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>287</v>
       </c>
@@ -4834,7 +4869,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>288</v>
       </c>
@@ -4845,7 +4880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>289</v>
       </c>
@@ -4856,7 +4891,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="20" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>290</v>
       </c>
@@ -4867,7 +4902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -4878,7 +4913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -4895,31 +4930,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7D8034F5-F038-4A88-A601-98CC4D69608C}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3 C5 C15:C18 C21:C22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE3D08DE-0C99-4CD2-8223-9013CFD55000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C4 C10:C11 C19:C20 C31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7E518415-2322-41FC-855A-3FB40C3BC649}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>C6:C9 C23:C30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D16BAC09-CAEC-43D5-9320-25A8CF7CC57C}">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>C12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{67C41D50-AA7D-45A0-B781-0061D0D7CB6E}">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
@@ -4932,7 +4967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD82E6C-E443-4C43-8643-8E84848061C8}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4940,12 +4975,12 @@
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -4953,67 +4988,67 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -5024,31 +5059,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F59A8D5D-A393-43F4-84C9-BF447EFC7A68}">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE3D8966-4A59-4DEA-A20D-9AC15BD1AFD0}">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C11ECD2-0203-4A95-A38B-283F848B1898}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>B6:B9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CF4AECF-E0BB-4CAE-B96C-B1762FD18C30}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B10:B11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE34ECD6-E16F-4201-A20B-33E78AF770A5}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
@@ -5061,7 +5096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8231F15-242A-43E7-9329-8D29896849C9}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5069,12 +5104,12 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
@@ -5082,137 +5117,137 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
         <v>290</v>
       </c>
       <c r="B23" s="20"/>
     </row>
-    <row r="24" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D8EFB88-1407-4DC4-A3DB-56CA143B999B}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B3 B7:B10 B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6256903-5087-4BC2-831D-B18268CDE6CD}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B5:B6 B11:B12 B23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CC30E241-3CB2-4609-ADDF-4B7243E7756F}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
change defaults data selections to ALL.  Update descriptions for data selection.
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW-Dev\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahamadeh\Dropbox\GitHub\OSP\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7342E41A-1AAA-46AA-9652-A50719A0A923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394913AC-7D9D-4C71-8C69-3CD9ED72BCF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="863" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="376">
   <si>
     <t>reportName</t>
   </si>
@@ -1008,12 +1008,6 @@
   </si>
   <si>
     <t>dataSelection</t>
-  </si>
-  <si>
-    <t>data selection filter for nonmem data file
-- ALL: all data selected
-- NONE: no data selected
-- R readable filter: data selection according to the filter</t>
   </si>
   <si>
     <t>dataDisplayName</t>
@@ -1435,9 +1429,6 @@
     <t>Plasma</t>
   </si>
   <si>
-    <t>Fraction Absorbed</t>
-  </si>
-  <si>
     <t>Active tasks</t>
   </si>
   <si>
@@ -1499,10 +1490,6 @@
   </si>
   <si>
     <t>display name of the observed data in report. Will be appended to the observed data display name of parent simulation set</t>
-  </si>
-  <si>
-    <t>data selection filter for nonmem data file (will be combined with SimSet data selection per &amp; )
-- R readable filter: data selection according to the filter</t>
   </si>
   <si>
     <t>Activity specific code</t>
@@ -1562,6 +1549,27 @@
   </si>
   <si>
     <t>Make sure 1=male 2= female</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>data selection filter for nonmem data file (will be combined with SimSet data selection per &amp; ).  Allowable inputs:
+- R readable filter
+- ALL: all data selected
+- NONE: no data selected
+- If left empty, no data are selected
+- R readable filter: data selection according to the filter</t>
+  </si>
+  <si>
+    <t>data selection filter for nonmem data file.  Allowable inputs:
+- ALL: all data selected
+- NONE: no data selected
+- If left empty, no data are selected
+- R readable filter: data selection according to the filter</t>
+  </si>
+  <si>
+    <t>Fraction Absorbed</t>
   </si>
 </sst>
 </file>
@@ -1738,9 +1746,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1755,12 +1760,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1775,9 +1774,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1793,7 +1801,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2117,12 +2125,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.09765625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>96</v>
       </c>
@@ -2130,7 +2138,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>97</v>
       </c>
@@ -2138,7 +2146,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
@@ -2158,24 +2166,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2190,16 +2198,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="48.09765625" customWidth="1"/>
+    <col min="7" max="7" width="48.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>53</v>
@@ -2220,7 +2228,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
@@ -2235,7 +2243,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>60</v>
       </c>
@@ -2250,7 +2258,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -2267,7 +2275,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>65</v>
       </c>
@@ -2284,7 +2292,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>68</v>
       </c>
@@ -2301,7 +2309,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>72</v>
       </c>
@@ -2322,7 +2330,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>78</v>
       </c>
@@ -2343,7 +2351,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>83</v>
       </c>
@@ -2364,7 +2372,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>88</v>
       </c>
@@ -2385,7 +2393,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>92</v>
       </c>
@@ -2403,10 +2411,10 @@
         <v>94</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>70</v>
       </c>
@@ -2435,15 +2443,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.3984375" customWidth="1"/>
-    <col min="2" max="2" width="18.296875" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
     <col min="4" max="4" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -2454,10 +2462,10 @@
         <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>80</v>
       </c>
@@ -2466,24 +2474,24 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>20</v>
       </c>
@@ -2491,13 +2499,13 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>20</v>
       </c>
@@ -2505,13 +2513,13 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>40</v>
       </c>
@@ -2519,13 +2527,13 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>40</v>
       </c>
@@ -2533,13 +2541,13 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>60</v>
       </c>
@@ -2564,21 +2572,21 @@
       <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>106</v>
       </c>
@@ -2610,13 +2618,13 @@
         <v>270</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -2648,13 +2656,13 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -2686,13 +2694,13 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>111</v>
       </c>
@@ -2712,10 +2720,10 @@
         <v>271</v>
       </c>
       <c r="L4" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>167</v>
       </c>
@@ -2732,10 +2740,10 @@
         <v>272</v>
       </c>
       <c r="L5" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>168</v>
       </c>
@@ -2749,10 +2757,10 @@
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>169</v>
       </c>
@@ -2766,10 +2774,10 @@
         <v>273</v>
       </c>
       <c r="L7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>170</v>
       </c>
@@ -2783,10 +2791,10 @@
         <v>269</v>
       </c>
       <c r="L8" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>171</v>
       </c>
@@ -2800,10 +2808,10 @@
         <v>274</v>
       </c>
       <c r="L9" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>172</v>
       </c>
@@ -2814,7 +2822,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>173</v>
       </c>
@@ -2825,7 +2833,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>174</v>
       </c>
@@ -2836,7 +2844,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>175</v>
       </c>
@@ -2847,7 +2855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>176</v>
       </c>
@@ -2858,7 +2866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>177</v>
       </c>
@@ -2869,7 +2877,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>178</v>
       </c>
@@ -2880,7 +2888,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>179</v>
       </c>
@@ -2891,7 +2899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>180</v>
       </c>
@@ -2902,7 +2910,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>181</v>
       </c>
@@ -2913,7 +2921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>182</v>
       </c>
@@ -2924,7 +2932,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>183</v>
       </c>
@@ -2935,7 +2943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>184</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>185</v>
       </c>
@@ -2954,7 +2962,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>186</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
         <v>187</v>
       </c>
@@ -2970,7 +2978,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>188</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>189</v>
       </c>
@@ -2986,7 +2994,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>190</v>
       </c>
@@ -2994,7 +3002,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>191</v>
       </c>
@@ -3002,42 +3010,42 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>239</v>
       </c>
@@ -3052,20 +3060,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFA2222-53E9-4EC9-97BD-22D97A0BEE05}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.19921875" customWidth="1"/>
-    <col min="3" max="3" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.69921875" customWidth="1"/>
+    <col min="2" max="2" width="100.25" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -3076,7 +3084,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>103</v>
       </c>
@@ -3087,7 +3095,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>104</v>
       </c>
@@ -3098,27 +3106,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>133</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>135</v>
       </c>
@@ -3129,23 +3137,23 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>332</v>
-      </c>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>341</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>115</v>
       </c>
@@ -3156,7 +3164,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>117</v>
       </c>
@@ -3167,7 +3175,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>119</v>
       </c>
@@ -3178,7 +3186,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>121</v>
       </c>
@@ -3189,7 +3197,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>123</v>
       </c>
@@ -3200,7 +3208,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>125</v>
       </c>
@@ -3211,7 +3219,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>127</v>
       </c>
@@ -3222,7 +3230,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>128</v>
       </c>
@@ -3233,7 +3241,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>129</v>
       </c>
@@ -3244,14 +3252,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+    </row>
+    <row r="19" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>137</v>
       </c>
@@ -3260,7 +3268,7 @@
       </c>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>138</v>
       </c>
@@ -3271,7 +3279,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>142</v>
       </c>
@@ -3280,7 +3288,7 @@
       </c>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>143</v>
       </c>
@@ -3289,7 +3297,7 @@
       </c>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>145</v>
       </c>
@@ -3300,7 +3308,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>146</v>
       </c>
@@ -3309,7 +3317,7 @@
       </c>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>160</v>
       </c>
@@ -3318,7 +3326,7 @@
       </c>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>152</v>
       </c>
@@ -3327,7 +3335,7 @@
       </c>
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>153</v>
       </c>
@@ -3336,7 +3344,7 @@
       </c>
       <c r="C27" s="16"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>156</v>
       </c>
@@ -3345,7 +3353,7 @@
       </c>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>158</v>
       </c>
@@ -3354,19 +3362,19 @@
       </c>
       <c r="C29" s="16"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="1:3" ht="53.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+    </row>
+    <row r="31" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C31" s="16"/>
     </row>
@@ -3395,7 +3403,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{4DD5E394-DB56-4CF9-8843-782939E4B76D}">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
@@ -3412,7 +3420,7 @@
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C17</xm:sqref>
+          <xm:sqref>C6 C9:C17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{27F5C9CF-E08E-451A-BDCC-8583F3505D62}">
           <x14:formula1>
@@ -3426,12 +3434,6 @@
           </x14:formula1>
           <xm:sqref>C7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{9E033B59-45BC-49B0-98F7-A5778FCFAB02}">
-          <x14:formula1>
-            <xm:f>Lookup!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C6 C9:C16</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3444,220 +3446,225 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.8984375" customWidth="1"/>
-    <col min="2" max="2" width="42.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.796875" customWidth="1"/>
-    <col min="4" max="4" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="42.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>303</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="20" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>291</v>
-      </c>
-      <c r="C9" s="23"/>
-    </row>
-    <row r="10" spans="1:4" s="20" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>337</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>314</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>333</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-    </row>
-    <row r="14" spans="1:4" s="20" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="20" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>335</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>322</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="20" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3702,110 +3709,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="C2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="C4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>359</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="20" customFormat="1" ht="69" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:4" s="20" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="C6" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>361</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="20" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>295</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3828,21 +3840,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.69921875" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.8984375" customWidth="1"/>
+    <col min="11" max="11" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
@@ -3879,7 +3891,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -3890,7 +3902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3936,13 +3948,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
@@ -3953,7 +3965,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -3964,7 +3976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3975,7 +3987,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -3986,7 +3998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -3997,7 +4009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>205</v>
       </c>
@@ -4008,7 +4020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>240</v>
       </c>
@@ -4019,7 +4031,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -4041,7 +4053,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -4052,7 +4064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -4063,7 +4075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -4074,7 +4086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -4085,7 +4097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4096,7 +4108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>252</v>
       </c>
@@ -4107,7 +4119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>253</v>
       </c>
@@ -4118,7 +4130,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>254</v>
       </c>
@@ -4129,7 +4141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>255</v>
       </c>
@@ -4140,7 +4152,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>256</v>
       </c>
@@ -4151,7 +4163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>257</v>
       </c>
@@ -4162,7 +4174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>258</v>
       </c>
@@ -4173,7 +4185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>259</v>
       </c>
@@ -4184,7 +4196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>260</v>
       </c>
@@ -4195,7 +4207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>261</v>
       </c>
@@ -4206,7 +4218,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>262</v>
       </c>
@@ -4217,7 +4229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>263</v>
       </c>
@@ -4228,7 +4240,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>264</v>
       </c>
@@ -4239,7 +4251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>265</v>
       </c>
@@ -4250,7 +4262,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>266</v>
       </c>
@@ -4261,7 +4273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>267</v>
       </c>
@@ -4272,7 +4284,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>268</v>
       </c>
@@ -4283,7 +4295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -4294,7 +4306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -4310,24 +4322,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{7D8034F5-F038-4A88-A601-98CC4D69608C}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>C22</xm:sqref>
+          <xm:sqref>C2:C3 C5 C15:C18 C21:C22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{AE3D08DE-0C99-4CD2-8223-9013CFD55000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C31</xm:sqref>
+          <xm:sqref>C31 C4 C10:C11 C19:C20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{7E518415-2322-41FC-855A-3FB40C3BC649}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
-          <xm:sqref>C30</xm:sqref>
+          <xm:sqref>C6:C9 C23:C30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{D16BAC09-CAEC-43D5-9320-25A8CF7CC57C}">
           <x14:formula1>
@@ -4339,31 +4351,7 @@
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A9664D0C-5DE1-4585-A34B-E8BC9313894D}">
-          <x14:formula1>
-            <xm:f>Lookup!$E$2:$E$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2 C3 C5 C15 C16 C17 C18 C21</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{08C5A947-E2B8-4354-98A9-FB093DE7AC93}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4 C10 C11 C19 C20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{5014D03B-826A-49F8-B79B-37EC796008BA}">
-          <x14:formula1>
-            <xm:f>Lookup!$G$2:$G$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>C6 C7 C8 C9 C23 C24 C25 C26 C27 C28 C29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{3D206683-23D2-47DF-B615-7F376DC60EC0}">
-          <x14:formula1>
-            <xm:f>Lookup!$I$2:$I$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C13</xm:sqref>
+          <xm:sqref>C13:C14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4380,84 +4368,84 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4467,12 +4455,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{F59A8D5D-A393-43F4-84C9-BF447EFC7A68}">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B13:B14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{BE3D8966-4A59-4DEA-A20D-9AC15BD1AFD0}">
           <x14:formula1>
@@ -4484,43 +4472,19 @@
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B6:B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{9CF4AECF-E0BB-4CAE-B96C-B1762FD18C30}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B11</xm:sqref>
+          <xm:sqref>B4 B10:B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{CE34ECD6-E16F-4201-A20B-33E78AF770A5}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{EC8692CC-A0D9-4CCD-872D-5B59B25ED033}">
-          <x14:formula1>
-            <xm:f>Lookup!$E$2:$E$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{785901DD-C03A-46FD-A658-301970C72EEF}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4 B10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{76FA5320-69B8-4D88-8C11-59BBCFC23CE3}">
-          <x14:formula1>
-            <xm:f>Lookup!$G$2:$G$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6:B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{55A21443-3366-4C61-81A2-7D78C71CBCC0}">
-          <x14:formula1>
-            <xm:f>Lookup!$I$2:$I$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
+          <xm:sqref>B5 B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4537,175 +4501,157 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{8D8EFB88-1407-4DC4-A3DB-56CA143B999B}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B2:B3 B7:B10 B13:B14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A6256903-5087-4BC2-831D-B18268CDE6CD}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B23</xm:sqref>
+          <xm:sqref>B23 B4:B6 B11:B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{CC30E241-3CB2-4609-ADDF-4B7243E7756F}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
-          <xm:sqref>B22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{54D99DC9-1EFD-44FB-8FBD-4A493AB06883}">
-          <x14:formula1>
-            <xm:f>Lookup!$E$2:$E$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3 B7:B10 B13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A794DFD8-A6D5-44DF-8C05-FFB9D0002BCE}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B6 B11:B12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{1D2EE919-65ED-4670-A982-8D9FC873CF1D}">
-          <x14:formula1>
-            <xm:f>Lookup!$G$2:$G$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15:B21</xm:sqref>
+          <xm:sqref>B15:B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4719,30 +4665,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Excel issue 426 (#438)
* Update utilities-excel-input.R

* modify concatenation in cases of NONE, ALL and NA

* change defaults data selections to ALL.  Update descriptions for data selection.
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW-Dev\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahamadeh\Dropbox\GitHub\OSP\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7342E41A-1AAA-46AA-9652-A50719A0A923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394913AC-7D9D-4C71-8C69-3CD9ED72BCF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="863" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="376">
   <si>
     <t>reportName</t>
   </si>
@@ -1008,12 +1008,6 @@
   </si>
   <si>
     <t>dataSelection</t>
-  </si>
-  <si>
-    <t>data selection filter for nonmem data file
-- ALL: all data selected
-- NONE: no data selected
-- R readable filter: data selection according to the filter</t>
   </si>
   <si>
     <t>dataDisplayName</t>
@@ -1435,9 +1429,6 @@
     <t>Plasma</t>
   </si>
   <si>
-    <t>Fraction Absorbed</t>
-  </si>
-  <si>
     <t>Active tasks</t>
   </si>
   <si>
@@ -1499,10 +1490,6 @@
   </si>
   <si>
     <t>display name of the observed data in report. Will be appended to the observed data display name of parent simulation set</t>
-  </si>
-  <si>
-    <t>data selection filter for nonmem data file (will be combined with SimSet data selection per &amp; )
-- R readable filter: data selection according to the filter</t>
   </si>
   <si>
     <t>Activity specific code</t>
@@ -1562,6 +1549,27 @@
   </si>
   <si>
     <t>Make sure 1=male 2= female</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>data selection filter for nonmem data file (will be combined with SimSet data selection per &amp; ).  Allowable inputs:
+- R readable filter
+- ALL: all data selected
+- NONE: no data selected
+- If left empty, no data are selected
+- R readable filter: data selection according to the filter</t>
+  </si>
+  <si>
+    <t>data selection filter for nonmem data file.  Allowable inputs:
+- ALL: all data selected
+- NONE: no data selected
+- If left empty, no data are selected
+- R readable filter: data selection according to the filter</t>
+  </si>
+  <si>
+    <t>Fraction Absorbed</t>
   </si>
 </sst>
 </file>
@@ -1738,9 +1746,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1755,12 +1760,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1775,9 +1774,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1793,7 +1801,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2117,12 +2125,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.09765625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>96</v>
       </c>
@@ -2130,7 +2138,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>97</v>
       </c>
@@ -2138,7 +2146,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
@@ -2158,24 +2166,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2190,16 +2198,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="48.09765625" customWidth="1"/>
+    <col min="7" max="7" width="48.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>53</v>
@@ -2220,7 +2228,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
@@ -2235,7 +2243,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>60</v>
       </c>
@@ -2250,7 +2258,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -2267,7 +2275,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>65</v>
       </c>
@@ -2284,7 +2292,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>68</v>
       </c>
@@ -2301,7 +2309,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>72</v>
       </c>
@@ -2322,7 +2330,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>78</v>
       </c>
@@ -2343,7 +2351,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>83</v>
       </c>
@@ -2364,7 +2372,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>88</v>
       </c>
@@ -2385,7 +2393,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>92</v>
       </c>
@@ -2403,10 +2411,10 @@
         <v>94</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>70</v>
       </c>
@@ -2435,15 +2443,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.3984375" customWidth="1"/>
-    <col min="2" max="2" width="18.296875" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
     <col min="4" max="4" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
@@ -2454,10 +2462,10 @@
         <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>80</v>
       </c>
@@ -2466,24 +2474,24 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>20</v>
       </c>
@@ -2491,13 +2499,13 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>20</v>
       </c>
@@ -2505,13 +2513,13 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>40</v>
       </c>
@@ -2519,13 +2527,13 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>40</v>
       </c>
@@ -2533,13 +2541,13 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>60</v>
       </c>
@@ -2564,21 +2572,21 @@
       <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>106</v>
       </c>
@@ -2610,13 +2618,13 @@
         <v>270</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -2648,13 +2656,13 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -2686,13 +2694,13 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>111</v>
       </c>
@@ -2712,10 +2720,10 @@
         <v>271</v>
       </c>
       <c r="L4" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>167</v>
       </c>
@@ -2732,10 +2740,10 @@
         <v>272</v>
       </c>
       <c r="L5" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>168</v>
       </c>
@@ -2749,10 +2757,10 @@
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>169</v>
       </c>
@@ -2766,10 +2774,10 @@
         <v>273</v>
       </c>
       <c r="L7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>170</v>
       </c>
@@ -2783,10 +2791,10 @@
         <v>269</v>
       </c>
       <c r="L8" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>171</v>
       </c>
@@ -2800,10 +2808,10 @@
         <v>274</v>
       </c>
       <c r="L9" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>172</v>
       </c>
@@ -2814,7 +2822,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>173</v>
       </c>
@@ -2825,7 +2833,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>174</v>
       </c>
@@ -2836,7 +2844,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>175</v>
       </c>
@@ -2847,7 +2855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>176</v>
       </c>
@@ -2858,7 +2866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>177</v>
       </c>
@@ -2869,7 +2877,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>178</v>
       </c>
@@ -2880,7 +2888,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>179</v>
       </c>
@@ -2891,7 +2899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>180</v>
       </c>
@@ -2902,7 +2910,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>181</v>
       </c>
@@ -2913,7 +2921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>182</v>
       </c>
@@ -2924,7 +2932,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>183</v>
       </c>
@@ -2935,7 +2943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>184</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>185</v>
       </c>
@@ -2954,7 +2962,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>186</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
         <v>187</v>
       </c>
@@ -2970,7 +2978,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>188</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>189</v>
       </c>
@@ -2986,7 +2994,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>190</v>
       </c>
@@ -2994,7 +3002,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>191</v>
       </c>
@@ -3002,42 +3010,42 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>239</v>
       </c>
@@ -3052,20 +3060,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFA2222-53E9-4EC9-97BD-22D97A0BEE05}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.19921875" customWidth="1"/>
-    <col min="3" max="3" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.69921875" customWidth="1"/>
+    <col min="2" max="2" width="100.25" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -3076,7 +3084,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>103</v>
       </c>
@@ -3087,7 +3095,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>104</v>
       </c>
@@ -3098,27 +3106,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>133</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>135</v>
       </c>
@@ -3129,23 +3137,23 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>332</v>
-      </c>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>341</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>115</v>
       </c>
@@ -3156,7 +3164,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>117</v>
       </c>
@@ -3167,7 +3175,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>119</v>
       </c>
@@ -3178,7 +3186,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>121</v>
       </c>
@@ -3189,7 +3197,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>123</v>
       </c>
@@ -3200,7 +3208,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>125</v>
       </c>
@@ -3211,7 +3219,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>127</v>
       </c>
@@ -3222,7 +3230,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>128</v>
       </c>
@@ -3233,7 +3241,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>129</v>
       </c>
@@ -3244,14 +3252,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+    </row>
+    <row r="19" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>137</v>
       </c>
@@ -3260,7 +3268,7 @@
       </c>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>138</v>
       </c>
@@ -3271,7 +3279,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>142</v>
       </c>
@@ -3280,7 +3288,7 @@
       </c>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>143</v>
       </c>
@@ -3289,7 +3297,7 @@
       </c>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>145</v>
       </c>
@@ -3300,7 +3308,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>146</v>
       </c>
@@ -3309,7 +3317,7 @@
       </c>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>160</v>
       </c>
@@ -3318,7 +3326,7 @@
       </c>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>152</v>
       </c>
@@ -3327,7 +3335,7 @@
       </c>
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>153</v>
       </c>
@@ -3336,7 +3344,7 @@
       </c>
       <c r="C27" s="16"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>156</v>
       </c>
@@ -3345,7 +3353,7 @@
       </c>
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>158</v>
       </c>
@@ -3354,19 +3362,19 @@
       </c>
       <c r="C29" s="16"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="1:3" ht="53.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+    </row>
+    <row r="31" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C31" s="16"/>
     </row>
@@ -3395,7 +3403,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{4DD5E394-DB56-4CF9-8843-782939E4B76D}">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
@@ -3412,7 +3420,7 @@
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C17</xm:sqref>
+          <xm:sqref>C6 C9:C17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{27F5C9CF-E08E-451A-BDCC-8583F3505D62}">
           <x14:formula1>
@@ -3426,12 +3434,6 @@
           </x14:formula1>
           <xm:sqref>C7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{9E033B59-45BC-49B0-98F7-A5778FCFAB02}">
-          <x14:formula1>
-            <xm:f>Lookup!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C6 C9:C16</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3444,220 +3446,225 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.8984375" customWidth="1"/>
-    <col min="2" max="2" width="42.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.796875" customWidth="1"/>
-    <col min="4" max="4" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="42.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="20" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>303</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="20" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="20" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>291</v>
-      </c>
-      <c r="C9" s="23"/>
-    </row>
-    <row r="10" spans="1:4" s="20" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>337</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>314</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>333</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-    </row>
-    <row r="14" spans="1:4" s="20" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="20" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>335</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>322</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="20" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3702,110 +3709,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="C2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="C4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>359</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="20" customFormat="1" ht="69" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:4" s="20" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="C6" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>361</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="20" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>295</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3828,21 +3840,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.69921875" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.8984375" customWidth="1"/>
+    <col min="11" max="11" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
@@ -3879,7 +3891,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -3890,7 +3902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3936,13 +3948,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
@@ -3953,7 +3965,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -3964,7 +3976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3975,7 +3987,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -3986,7 +3998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -3997,7 +4009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>205</v>
       </c>
@@ -4008,7 +4020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>240</v>
       </c>
@@ -4019,7 +4031,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -4041,7 +4053,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -4052,7 +4064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -4063,7 +4075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -4074,7 +4086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -4085,7 +4097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4096,7 +4108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>252</v>
       </c>
@@ -4107,7 +4119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>253</v>
       </c>
@@ -4118,7 +4130,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>254</v>
       </c>
@@ -4129,7 +4141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>255</v>
       </c>
@@ -4140,7 +4152,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>256</v>
       </c>
@@ -4151,7 +4163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>257</v>
       </c>
@@ -4162,7 +4174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>258</v>
       </c>
@@ -4173,7 +4185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>259</v>
       </c>
@@ -4184,7 +4196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>260</v>
       </c>
@@ -4195,7 +4207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>261</v>
       </c>
@@ -4206,7 +4218,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>262</v>
       </c>
@@ -4217,7 +4229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>263</v>
       </c>
@@ -4228,7 +4240,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>264</v>
       </c>
@@ -4239,7 +4251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>265</v>
       </c>
@@ -4250,7 +4262,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>266</v>
       </c>
@@ -4261,7 +4273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>267</v>
       </c>
@@ -4272,7 +4284,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>268</v>
       </c>
@@ -4283,7 +4295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -4294,7 +4306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -4310,24 +4322,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{7D8034F5-F038-4A88-A601-98CC4D69608C}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>C22</xm:sqref>
+          <xm:sqref>C2:C3 C5 C15:C18 C21:C22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{AE3D08DE-0C99-4CD2-8223-9013CFD55000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C31</xm:sqref>
+          <xm:sqref>C31 C4 C10:C11 C19:C20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{7E518415-2322-41FC-855A-3FB40C3BC649}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
-          <xm:sqref>C30</xm:sqref>
+          <xm:sqref>C6:C9 C23:C30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{D16BAC09-CAEC-43D5-9320-25A8CF7CC57C}">
           <x14:formula1>
@@ -4339,31 +4351,7 @@
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A9664D0C-5DE1-4585-A34B-E8BC9313894D}">
-          <x14:formula1>
-            <xm:f>Lookup!$E$2:$E$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2 C3 C5 C15 C16 C17 C18 C21</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{08C5A947-E2B8-4354-98A9-FB093DE7AC93}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4 C10 C11 C19 C20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{5014D03B-826A-49F8-B79B-37EC796008BA}">
-          <x14:formula1>
-            <xm:f>Lookup!$G$2:$G$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>C6 C7 C8 C9 C23 C24 C25 C26 C27 C28 C29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{3D206683-23D2-47DF-B615-7F376DC60EC0}">
-          <x14:formula1>
-            <xm:f>Lookup!$I$2:$I$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C13</xm:sqref>
+          <xm:sqref>C13:C14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4380,84 +4368,84 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4467,12 +4455,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{F59A8D5D-A393-43F4-84C9-BF447EFC7A68}">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B13:B14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{BE3D8966-4A59-4DEA-A20D-9AC15BD1AFD0}">
           <x14:formula1>
@@ -4484,43 +4472,19 @@
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B6:B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{9CF4AECF-E0BB-4CAE-B96C-B1762FD18C30}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B11</xm:sqref>
+          <xm:sqref>B4 B10:B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{CE34ECD6-E16F-4201-A20B-33E78AF770A5}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{EC8692CC-A0D9-4CCD-872D-5B59B25ED033}">
-          <x14:formula1>
-            <xm:f>Lookup!$E$2:$E$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{785901DD-C03A-46FD-A658-301970C72EEF}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4 B10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{76FA5320-69B8-4D88-8C11-59BBCFC23CE3}">
-          <x14:formula1>
-            <xm:f>Lookup!$G$2:$G$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6:B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{55A21443-3366-4C61-81A2-7D78C71CBCC0}">
-          <x14:formula1>
-            <xm:f>Lookup!$I$2:$I$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
+          <xm:sqref>B5 B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4537,175 +4501,157 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{8D8EFB88-1407-4DC4-A3DB-56CA143B999B}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B2:B3 B7:B10 B13:B14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A6256903-5087-4BC2-831D-B18268CDE6CD}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B23</xm:sqref>
+          <xm:sqref>B23 B4:B6 B11:B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{CC30E241-3CB2-4609-ADDF-4B7243E7756F}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
-          <xm:sqref>B22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{54D99DC9-1EFD-44FB-8FBD-4A493AB06883}">
-          <x14:formula1>
-            <xm:f>Lookup!$E$2:$E$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3 B7:B10 B13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A794DFD8-A6D5-44DF-8C05-FFB9D0002BCE}">
-          <x14:formula1>
-            <xm:f>Lookup!$F$2:$F$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B6 B11:B12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{1D2EE919-65ED-4670-A982-8D9FC873CF1D}">
-          <x14:formula1>
-            <xm:f>Lookup!$G$2:$G$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15:B21</xm:sqref>
+          <xm:sqref>B15:B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4719,30 +4665,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
remove simulationName #415 (#441)
* remove simulationName #415

* update documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahamadeh\Dropbox\GitHub\OSP\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394913AC-7D9D-4C71-8C69-3CD9ED72BCF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ECC2A6-C386-489E-9629-5FA77ADB1487}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="863" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="863" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="374">
   <si>
     <t>reportName</t>
   </si>
@@ -1032,12 +1032,6 @@
   </si>
   <si>
     <t>simulationFile</t>
-  </si>
-  <si>
-    <t>simulationName</t>
-  </si>
-  <si>
-    <t>display name of simulation for report</t>
   </si>
   <si>
     <t>Outputs_1</t>
@@ -2173,17 +2167,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2201,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>53</v>
@@ -2411,7 +2405,7 @@
         <v>94</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2462,7 +2456,7 @@
         <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2474,21 +2468,21 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>366</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2499,7 +2493,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2513,7 +2507,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -2527,7 +2521,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -2541,7 +2535,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -2618,10 +2612,10 @@
         <v>270</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2656,10 +2650,10 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2694,10 +2688,10 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2720,7 +2714,7 @@
         <v>271</v>
       </c>
       <c r="L4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2740,7 +2734,7 @@
         <v>272</v>
       </c>
       <c r="L5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2757,7 +2751,7 @@
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2774,7 +2768,7 @@
         <v>273</v>
       </c>
       <c r="L7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2791,7 +2785,7 @@
         <v>269</v>
       </c>
       <c r="L8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2808,7 +2802,7 @@
         <v>274</v>
       </c>
       <c r="L9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3062,7 +3056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3111,7 +3105,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>134</v>
@@ -3119,10 +3113,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -3139,16 +3133,16 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -3254,7 +3248,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
@@ -3364,17 +3358,17 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C31" s="16"/>
     </row>
@@ -3384,7 +3378,7 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A30:C30"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19 C21 C26" xr:uid="{9AAEE111-A552-4065-B73D-436FB9662F75}">
       <formula1>1</formula1>
     </dataValidation>
@@ -3403,7 +3397,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{4DD5E394-DB56-4CF9-8843-782939E4B76D}">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
@@ -3442,11 +3436,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BE365A-43FF-4890-B212-B66C20B6B64E}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3465,10 +3459,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3484,123 +3478,123 @@
         <v>298</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="D4" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>4</v>
-      </c>
       <c r="B5" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B6" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="19" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>309</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>306</v>
+        <v>303</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>322</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>307</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>337</v>
+        <v>310</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>332</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="B13" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-    </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>315</v>
       </c>
@@ -3608,21 +3602,25 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>317</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C15" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>319</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>320</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="B16" s="20"/>
       <c r="C16" s="19" t="s">
         <v>141</v>
       </c>
@@ -3632,44 +3630,32 @@
     </row>
     <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>334</v>
-      </c>
-      <c r="B17" s="20"/>
+        <v>319</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>321</v>
+      </c>
       <c r="C17" s="19" t="s">
-        <v>141</v>
+        <v>304</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="B18" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>306</v>
-      </c>
       <c r="D18" s="19" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
-        <v>322</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>325</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1" xr:uid="{2F698D61-A5E7-4592-8B8E-273A452D2878}">
@@ -3685,19 +3671,19 @@
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:D7 C18:D18</xm:sqref>
+          <xm:sqref>C6:D6 C17:D17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{6EF3833C-AEDC-4515-860C-DDCECEDDAE3A}">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C16:D17</xm:sqref>
+          <xm:sqref>C15:D16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{8B42858B-1E8D-4E92-BA09-9641651F1D9E}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C11:D11</xm:sqref>
+          <xm:sqref>C10:D10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3709,7 +3695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
@@ -3730,10 +3716,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3741,7 +3727,7 @@
         <v>288</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -3769,7 +3755,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -3783,13 +3769,13 @@
         <v>290</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -3797,13 +3783,13 @@
         <v>291</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixes #533 add third option for dataUnit
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahamadeh\Dropbox\GitHub\OSP\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F23466-96F3-4C41-B38A-221098DFA30D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <sheet name="StudyDesign" sheetId="21" r:id="rId12"/>
     <sheet name="Lookup" sheetId="16" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="378">
   <si>
     <t>reportName</t>
   </si>
@@ -1571,11 +1570,17 @@
   <si>
     <t>Optional alternative name for 'simulation set', to be used in reports.</t>
   </si>
+  <si>
+    <t>dataUnit</t>
+  </si>
+  <si>
+    <t>unit of corresponding observed data in dataset</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1876,23 +1881,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1928,23 +1916,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2120,7 +2091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2161,7 +2132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2193,7 +2164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2438,7 +2409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFAFC31-38D5-48B3-9906-8E611B925363}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2564,7 +2535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39160AF7-ED4A-459F-ABF7-9A3E8B4E93E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3057,10 +3028,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFA2222-53E9-4EC9-97BD-22D97A0BEE05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="A7:C7"/>
     </sheetView>
@@ -3394,51 +3365,51 @@
     <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C22 C27" xr:uid="{9AAEE111-A552-4065-B73D-436FB9662F75}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C22 C27">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{A3853C53-84A6-406F-8D51-D6DB90939D8F}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28" xr:uid="{FBF9A4B6-7740-472B-BDC7-E4094280D0C9}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30" xr:uid="{9DA068F6-BC04-485B-84BE-0C4A8052EF05}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C7" xr:uid="{115CEB48-16B3-43AC-A742-B81FC51DA635}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{4DD5E394-DB56-4CF9-8843-782939E4B76D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{41782F69-4DE6-4E69-99A4-8E5A162A7617}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{6C9B617F-76A5-4A18-8C52-8FC6FCDC5553}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>C10:C18 C6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{27F5C9CF-E08E-451A-BDCC-8583F3505D62}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>C21 C23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F52AC8F-74E3-4321-8F38-3FEDED88C0D8}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$L$2:$L$9</xm:f>
           </x14:formula1>
@@ -3451,7 +3422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BE365A-43FF-4890-B212-B66C20B6B64E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3674,7 +3645,7 @@
     <mergeCell ref="A12:D12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1" xr:uid="{2F698D61-A5E7-4592-8B8E-273A452D2878}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3683,19 +3654,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{5EFC9B10-DECD-48CD-8E33-903B2F25A5CD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>C6:D6 C17:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{6EF3833C-AEDC-4515-860C-DDCECEDDAE3A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>C15:D16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{8B42858B-1E8D-4E92-BA09-9641651F1D9E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
@@ -3708,12 +3679,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3810,21 +3781,30 @@
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="C7" s="28"/>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B8" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C8" s="29" t="s">
         <v>293</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D8" s="29" t="s">
         <v>294</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1" xr:uid="{24357576-89E4-4315-AA8F-C7BBB658C748}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3834,7 +3814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1C5AA6-6C28-45A7-A61F-94EA6ED12211}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3917,10 +3897,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100 F2:G100 I2:I100 K2:K100" xr:uid="{207A22CC-5202-403D-BEA7-EB15D62C21E4}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100 F2:G100 I2:I100 K2:K100">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E100 H2:H100" xr:uid="{AFED9A83-72E8-4C71-9E41-7C51A4947FEA}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E100 H2:H100">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -3929,7 +3909,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{3F8A55C5-1413-4609-A2FB-C839F38EB0B4}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$J$2:$J$22</xm:f>
           </x14:formula1>
@@ -3942,7 +3922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB85399-C384-4052-AD23-5D6464C511C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4325,31 +4305,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{7D8034F5-F038-4A88-A601-98CC4D69608C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3 C5 C15:C18 C21:C22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{AE3D08DE-0C99-4CD2-8223-9013CFD55000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C31 C4 C10:C11 C19:C20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{7E518415-2322-41FC-855A-3FB40C3BC649}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>C6:C9 C23:C30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{D16BAC09-CAEC-43D5-9320-25A8CF7CC57C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>C12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{67C41D50-AA7D-45A0-B781-0061D0D7CB6E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
@@ -4362,7 +4342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD82E6C-E443-4C43-8643-8E84848061C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4458,31 +4438,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{F59A8D5D-A393-43F4-84C9-BF447EFC7A68}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{BE3D8966-4A59-4DEA-A20D-9AC15BD1AFD0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{9C11ECD2-0203-4A95-A38B-283F848B1898}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>B6:B9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{9CF4AECF-E0BB-4CAE-B96C-B1762FD18C30}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B10:B11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{CE34ECD6-E16F-4201-A20B-33E78AF770A5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
@@ -4495,7 +4475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8231F15-242A-43E7-9329-8D29896849C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4637,19 +4617,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{8D8EFB88-1407-4DC4-A3DB-56CA143B999B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B3 B7:B10 B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{A6256903-5087-4BC2-831D-B18268CDE6CD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B23 B4:B6 B11:B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{CC30E241-3CB2-4609-ADDF-4B7243E7756F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
@@ -4662,7 +4642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B262A-9A5B-46FC-A725-85413523FCCF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixes #540 option for including reference data is translated
The option seemed only for observed data (quid of simulations and related residuals) and specific to simulation set.
However, I currently define it at the workflow level which made more sense to me.
Thus, I have renamed, moved and linked the option to the task setting `includeReferenceData`
Let me know if that makes sense
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="379">
   <si>
     <t>reportName</t>
   </si>
@@ -1402,9 +1402,6 @@
     <t>simulation start offset</t>
   </si>
   <si>
-    <t>plotReferenceObsData</t>
-  </si>
-  <si>
     <t>display name of the observed data in report. Will be concatenated with the output display name</t>
   </si>
   <si>
@@ -1575,6 +1572,24 @@
   </si>
   <si>
     <t>unit of corresponding observed data in dataset</t>
+  </si>
+  <si>
+    <t>plotTimeProfilesAndResiduals: includeReferenceData</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"plotTimeProfilesAndResiduals" task: Include data from reference population in other simulationSets results. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Relevant for POPULATION workflow of type pediatric and ratioComparison only.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2382,7 +2397,7 @@
         <v>94</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2433,7 +2448,7 @@
         <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,21 +2460,21 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2470,7 +2485,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2484,7 +2499,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -2498,7 +2513,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -2512,7 +2527,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -2592,7 +2607,7 @@
         <v>305</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2630,7 +2645,7 @@
         <v>303</v>
       </c>
       <c r="L2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2668,7 +2683,7 @@
         <v>304</v>
       </c>
       <c r="L3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2691,7 +2706,7 @@
         <v>270</v>
       </c>
       <c r="L4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2711,7 +2726,7 @@
         <v>271</v>
       </c>
       <c r="L5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2728,7 +2743,7 @@
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2745,7 +2760,7 @@
         <v>272</v>
       </c>
       <c r="L7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2762,7 +2777,7 @@
         <v>268</v>
       </c>
       <c r="L8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2779,7 +2794,7 @@
         <v>273</v>
       </c>
       <c r="L9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3029,11 +3044,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3060,7 +3075,7 @@
         <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>108</v>
@@ -3090,10 +3105,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>338</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>339</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -3110,10 +3125,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>374</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>375</v>
       </c>
       <c r="C7" s="16"/>
     </row>
@@ -3128,7 +3143,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -3234,7 +3249,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -3308,74 +3323,85 @@
     </row>
     <row r="27" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="C27" s="16"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B31" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+    </row>
+    <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-    </row>
-    <row r="32" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
+      <c r="B33" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="C32" s="16"/>
+      <c r="C33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C22 C27">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C22 C28">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C31">
       <formula1>2</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C7"/>
@@ -3407,7 +3433,7 @@
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C21 C23</xm:sqref>
+          <xm:sqref>C21 C23 C27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -3423,11 +3449,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3446,10 +3472,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>349</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3520,13 +3546,13 @@
         <v>289</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3534,13 +3560,13 @@
         <v>290</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>333</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3605,39 +3631,27 @@
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>331</v>
-      </c>
-      <c r="B16" s="20"/>
+        <v>318</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>320</v>
+      </c>
       <c r="C16" s="19" t="s">
-        <v>140</v>
+        <v>303</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>318</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>320</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>303</v>
+        <v>319</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>322</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>319</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>322</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3658,13 +3672,13 @@
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:D6 C17:D17</xm:sqref>
+          <xm:sqref>C6:D6 C16:D16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C15:D16</xm:sqref>
+          <xm:sqref>C15:D15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
@@ -3682,7 +3696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -3703,10 +3717,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>352</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3714,7 +3728,7 @@
         <v>287</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -3742,7 +3756,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -3756,13 +3770,13 @@
         <v>289</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -3770,21 +3784,21 @@
         <v>290</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>376</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>377</v>
       </c>
       <c r="C7" s="28"/>
     </row>

</xml_diff>

<commit_message>
Fixes #540 plotReferenceObsData from Excel template taken into accounted
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="379">
   <si>
     <t>reportName</t>
   </si>
@@ -1237,9 +1237,6 @@
     <t>referencePopulation</t>
   </si>
   <si>
-    <t>reference population used in Pediatric and Ratio Comparison workflows</t>
-  </si>
-  <si>
     <t>StudyDesignType</t>
   </si>
   <si>
@@ -1575,6 +1572,12 @@
   </si>
   <si>
     <t>unit of corresponding observed data in dataset</t>
+  </si>
+  <si>
+    <t>Reference population used in Pediatric and Ratio Comparison workflows</t>
+  </si>
+  <si>
+    <t>Observed data from reference population is plotted in a Simulation Set time profiles of Pediatric and Ratio Comparison workflows</t>
   </si>
 </sst>
 </file>
@@ -2144,17 +2147,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2178,7 +2181,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>53</v>
@@ -2382,7 +2385,7 @@
         <v>94</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2433,7 +2436,7 @@
         <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,21 +2448,21 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2470,7 +2473,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2484,7 +2487,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -2498,7 +2501,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -2512,7 +2515,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -2592,7 +2595,7 @@
         <v>305</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2630,7 +2633,7 @@
         <v>303</v>
       </c>
       <c r="L2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2668,7 +2671,7 @@
         <v>304</v>
       </c>
       <c r="L3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2691,7 +2694,7 @@
         <v>270</v>
       </c>
       <c r="L4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2711,7 +2714,7 @@
         <v>271</v>
       </c>
       <c r="L5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2728,7 +2731,7 @@
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2745,7 +2748,7 @@
         <v>272</v>
       </c>
       <c r="L7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2762,7 +2765,7 @@
         <v>268</v>
       </c>
       <c r="L8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2779,7 +2782,7 @@
         <v>273</v>
       </c>
       <c r="L9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3060,7 +3063,7 @@
         <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>108</v>
@@ -3090,10 +3093,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>338</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>339</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -3110,25 +3113,25 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>374</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>375</v>
       </c>
       <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>327</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>328</v>
       </c>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -3234,7 +3237,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -3344,17 +3347,17 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
     </row>
     <row r="32" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>358</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>359</v>
       </c>
       <c r="C32" s="16"/>
     </row>
@@ -3425,9 +3428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3446,10 +3449,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>349</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3509,7 +3512,7 @@
         <v>302</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>95</v>
@@ -3520,13 +3523,13 @@
         <v>289</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3534,13 +3537,13 @@
         <v>290</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>333</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3559,10 +3562,10 @@
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>329</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3594,7 +3597,7 @@
         <v>316</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>140</v>
@@ -3603,11 +3606,13 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>331</v>
-      </c>
-      <c r="B16" s="20"/>
+        <v>330</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>378</v>
+      </c>
       <c r="C16" s="19" t="s">
         <v>140</v>
       </c>
@@ -3617,10 +3622,10 @@
     </row>
     <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>303</v>
@@ -3631,13 +3636,13 @@
     </row>
     <row r="18" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3682,7 +3687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -3703,10 +3708,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>352</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3714,7 +3719,7 @@
         <v>287</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -3742,7 +3747,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -3756,13 +3761,13 @@
         <v>289</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -3770,21 +3775,21 @@
         <v>290</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>376</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>377</v>
       </c>
       <c r="C7" s="28"/>
     </row>

</xml_diff>

<commit_message>
540 ref obs data (#647)
* Fixes #540 Population simulation sets include plotReferenceObsData

* Fixes #540 plotReferenceObsData from Excel template taken into accounted

* Fix logic of reference data inclusion at the task level
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="379">
   <si>
     <t>reportName</t>
   </si>
@@ -1237,9 +1237,6 @@
     <t>referencePopulation</t>
   </si>
   <si>
-    <t>reference population used in Pediatric and Ratio Comparison workflows</t>
-  </si>
-  <si>
     <t>StudyDesignType</t>
   </si>
   <si>
@@ -1575,6 +1572,12 @@
   </si>
   <si>
     <t>unit of corresponding observed data in dataset</t>
+  </si>
+  <si>
+    <t>Reference population used in Pediatric and Ratio Comparison workflows</t>
+  </si>
+  <si>
+    <t>Observed data from reference population is plotted in a Simulation Set time profiles of Pediatric and Ratio Comparison workflows</t>
   </si>
 </sst>
 </file>
@@ -2144,17 +2147,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2178,7 +2181,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>53</v>
@@ -2382,7 +2385,7 @@
         <v>94</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2433,7 +2436,7 @@
         <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,21 +2448,21 @@
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2470,7 +2473,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2484,7 +2487,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -2498,7 +2501,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -2512,7 +2515,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -2592,7 +2595,7 @@
         <v>305</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2630,7 +2633,7 @@
         <v>303</v>
       </c>
       <c r="L2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2668,7 +2671,7 @@
         <v>304</v>
       </c>
       <c r="L3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2691,7 +2694,7 @@
         <v>270</v>
       </c>
       <c r="L4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2711,7 +2714,7 @@
         <v>271</v>
       </c>
       <c r="L5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2728,7 +2731,7 @@
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2745,7 +2748,7 @@
         <v>272</v>
       </c>
       <c r="L7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2762,7 +2765,7 @@
         <v>268</v>
       </c>
       <c r="L8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2779,7 +2782,7 @@
         <v>273</v>
       </c>
       <c r="L9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -3060,7 +3063,7 @@
         <v>103</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>108</v>
@@ -3090,10 +3093,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>338</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>339</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -3110,25 +3113,25 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>374</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>375</v>
       </c>
       <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>327</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>328</v>
       </c>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -3234,7 +3237,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -3344,17 +3347,17 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
     </row>
     <row r="32" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>358</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>359</v>
       </c>
       <c r="C32" s="16"/>
     </row>
@@ -3425,9 +3428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3446,10 +3449,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>349</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3509,7 +3512,7 @@
         <v>302</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>95</v>
@@ -3520,13 +3523,13 @@
         <v>289</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3534,13 +3537,13 @@
         <v>290</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>333</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3559,10 +3562,10 @@
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>329</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3594,7 +3597,7 @@
         <v>316</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>140</v>
@@ -3603,11 +3606,13 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>331</v>
-      </c>
-      <c r="B16" s="20"/>
+        <v>330</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>378</v>
+      </c>
       <c r="C16" s="19" t="s">
         <v>140</v>
       </c>
@@ -3617,10 +3622,10 @@
     </row>
     <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>303</v>
@@ -3631,13 +3636,13 @@
     </row>
     <row r="18" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3682,7 +3687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -3703,10 +3708,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>352</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -3714,7 +3719,7 @@
         <v>287</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -3742,7 +3747,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -3756,13 +3761,13 @@
         <v>289</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -3770,21 +3775,21 @@
         <v>290</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>376</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>377</v>
       </c>
       <c r="C7" s="28"/>
     </row>

</xml_diff>

<commit_message>
Integrate timeOffset in excel template
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -3036,7 +3036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="A7:C7"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3429,8 +3429,8 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3566,6 +3566,12 @@
       </c>
       <c r="B11" s="20" t="s">
         <v>329</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
313 time offset (#651)
* Fixes #313 time offset variable in simulation set for shifting time

While fixing this issue, I imported ospsuite.utils in NAMESPACE so ospsuite.utils:: should not be necessary any longer

* Integrate timeOffset in excel template

* Document timeOffset in vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -3036,7 +3036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="A7:C7"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3429,8 +3429,8 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3566,6 +3566,12 @@
       </c>
       <c r="B11" s="20" t="s">
         <v>329</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixes #855, #870, #873, #882 Excel template accounts for new features
New features include:
- DataSource objects
- Output new parameters
- Workflow title
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="2"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
     <sheet name="Workflow and Tasks" sheetId="13" r:id="rId2"/>
     <sheet name="SimulationSets" sheetId="20" r:id="rId3"/>
-    <sheet name="Outputs_1" sheetId="5" r:id="rId4"/>
-    <sheet name="Userdef PK Parameter" sheetId="15" r:id="rId5"/>
-    <sheet name="PK Parameter" sheetId="14" r:id="rId6"/>
-    <sheet name="PK Conc Single" sheetId="17" r:id="rId7"/>
-    <sheet name="PK Conc Multi" sheetId="18" r:id="rId8"/>
-    <sheet name="PK Fraction" sheetId="19" r:id="rId9"/>
-    <sheet name="SensitivityParameter" sheetId="7" r:id="rId10"/>
-    <sheet name="tpDictionary" sheetId="11" r:id="rId11"/>
-    <sheet name="StudyDesign" sheetId="21" r:id="rId12"/>
-    <sheet name="Lookup" sheetId="16" r:id="rId13"/>
+    <sheet name="Outputs" sheetId="5" r:id="rId4"/>
+    <sheet name="Data Sources" sheetId="22" r:id="rId5"/>
+    <sheet name="Userdef PK Parameter" sheetId="15" r:id="rId6"/>
+    <sheet name="PK Parameter" sheetId="14" r:id="rId7"/>
+    <sheet name="PK Conc Single" sheetId="17" r:id="rId8"/>
+    <sheet name="PK Conc Multi" sheetId="18" r:id="rId9"/>
+    <sheet name="PK Fraction" sheetId="19" r:id="rId10"/>
+    <sheet name="SensitivityParameter" sheetId="7" r:id="rId11"/>
+    <sheet name="tpDictionary" sheetId="11" r:id="rId12"/>
+    <sheet name="StudyDesign" sheetId="21" r:id="rId13"/>
+    <sheet name="Lookup" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="415">
   <si>
     <t>reportName</t>
   </si>
@@ -199,9 +200,6 @@
     <t>Thalf_tLast_tEnd</t>
   </si>
   <si>
-    <t>name of the sheet with the output definitions</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -446,9 +444,6 @@
   </si>
   <si>
     <t>createWordReport</t>
-  </si>
-  <si>
-    <t>If activated: MS Word report will be created additionally to Markdon report</t>
   </si>
   <si>
     <t>simulate: numberOfCores</t>
@@ -1026,12 +1021,6 @@
   </si>
   <si>
     <t>simulationFile</t>
-  </si>
-  <si>
-    <t>Outputs_1</t>
-  </si>
-  <si>
-    <t>observedDataFile</t>
   </si>
   <si>
     <r>
@@ -1423,9 +1412,6 @@
     <t>reportFileName</t>
   </si>
   <si>
-    <t>Name of the report fille; keep empty to use the default</t>
-  </si>
-  <si>
     <t>PlotFormat</t>
   </si>
   <si>
@@ -1578,6 +1564,193 @@
   </si>
   <si>
     <t>Observed data from reference population is plotted in a Simulation Set time profiles of Pediatric and Ratio Comparison workflows</t>
+  </si>
+  <si>
+    <t>dataFile</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>Source1</t>
+  </si>
+  <si>
+    <t>Source2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Displayed data source caption in the report. The caption will be preceeded by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Data source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>groupID</t>
+  </si>
+  <si>
+    <t>identifier for splitting outputs by the combination {displayUnit; groupID}. Each combination becomes then a separate plot</t>
+  </si>
+  <si>
+    <t>reportTitle</t>
+  </si>
+  <si>
+    <t>Title included on top of the report</t>
+  </si>
+  <si>
+    <t>Output1, Output2</t>
+  </si>
+  <si>
+    <t>dataSource</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">name of included data sources defined in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Data Sources </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sheet</t>
+    </r>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>#5050FF</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>#CE3D32</t>
+  </si>
+  <si>
+    <t>#749B58</t>
+  </si>
+  <si>
+    <t>#F0E685</t>
+  </si>
+  <si>
+    <t>#466983</t>
+  </si>
+  <si>
+    <t>#BA6338</t>
+  </si>
+  <si>
+    <t>#5DB1DD</t>
+  </si>
+  <si>
+    <t>#802268</t>
+  </si>
+  <si>
+    <t>#6BD76B</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>magenta</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">name of included outputs defined in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Outputs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet. Separate outputs with a coma to include multiple outputs</t>
+    </r>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>maroon</t>
+  </si>
+  <si>
+    <t>olive</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>navy</t>
+  </si>
+  <si>
+    <t>display color in plots</t>
+  </si>
+  <si>
+    <t>If activated: MS Word report will be created additionally to Markdown report</t>
+  </si>
+  <si>
+    <t>Name of the report file. Remember to include Markdown .md extension. Keep empty to use the default</t>
+  </si>
+  <si>
+    <t>a.md</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1782,6 +1955,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1795,8 +1969,744 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="103">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5050FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCE3D32"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF749B58"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF0E685"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF008000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF466983"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000080"/>
+      <color rgb="FF800080"/>
+      <color rgb="FF808000"/>
+      <color rgb="FF800000"/>
+      <color rgb="FF808080"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF008000"/>
+      <color rgb="FF6BD76B"/>
+      <color rgb="FF802268"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2097,7 +3007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2106,26 +3016,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2135,6 +3045,47 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -2147,17 +3098,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -2181,16 +3132,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -2199,18 +3150,18 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2219,13 +3170,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2234,13 +3185,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -2251,30 +3202,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>18</v>
@@ -2285,124 +3236,124 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>94</v>
-      </c>
       <c r="G11" s="9" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +3362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2427,42 +3378,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2473,7 +3424,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2487,7 +3438,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -2501,7 +3452,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -2515,7 +3466,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -2537,13 +3488,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2560,106 +3511,112 @@
     <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>249</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="L2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
@@ -2668,340 +3625,400 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="L3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+      <c r="M3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+      <c r="M4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="M5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+      <c r="M6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
       </c>
       <c r="J7" t="s">
+        <v>270</v>
+      </c>
+      <c r="L7" t="s">
+        <v>342</v>
+      </c>
+      <c r="M7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" t="s">
+        <v>266</v>
+      </c>
+      <c r="L8" t="s">
+        <v>340</v>
+      </c>
+      <c r="M8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" t="s">
+        <v>271</v>
+      </c>
+      <c r="L9" t="s">
+        <v>341</v>
+      </c>
+      <c r="M9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G10" t="s">
+        <v>211</v>
+      </c>
+      <c r="J10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G11" t="s">
+        <v>212</v>
+      </c>
+      <c r="J11" t="s">
+        <v>237</v>
+      </c>
+      <c r="M11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" t="s">
+        <v>213</v>
+      </c>
+      <c r="J12" t="s">
         <v>272</v>
       </c>
-      <c r="L7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J8" t="s">
-        <v>268</v>
-      </c>
-      <c r="L8" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F9" t="s">
-        <v>202</v>
-      </c>
-      <c r="G9" t="s">
-        <v>212</v>
-      </c>
-      <c r="J9" t="s">
-        <v>273</v>
-      </c>
-      <c r="L9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E10" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" t="s">
-        <v>213</v>
-      </c>
-      <c r="J10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
+      <c r="M12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
         <v>172</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G13" t="s">
         <v>214</v>
-      </c>
-      <c r="J11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E12" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" t="s">
-        <v>215</v>
-      </c>
-      <c r="J12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" t="s">
-        <v>216</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+      <c r="M15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+      <c r="M16" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+      <c r="M18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G22" t="s">
+        <v>222</v>
+      </c>
+      <c r="J22" t="s">
+        <v>276</v>
+      </c>
+      <c r="M22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
         <v>183</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G24" t="s">
         <v>224</v>
       </c>
-      <c r="J22" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E23" t="s">
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
         <v>184</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E24" t="s">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
         <v>185</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E25" t="s">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
         <v>186</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
         <v>187</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G28" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E27" t="s">
+    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
         <v>188</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" t="s">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G29" t="s">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G30" t="s">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G32" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.2">
@@ -3011,17 +4028,17 @@
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3032,11 +4049,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3055,26 +4072,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>3</v>
@@ -3082,312 +4099,355 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>337</v>
+        <v>381</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>338</v>
+        <v>382</v>
       </c>
       <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>134</v>
+        <v>333</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>135</v>
+        <v>413</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>112</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>373</v>
+        <v>133</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="C7" s="16"/>
+        <v>412</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>327</v>
+        <v>369</v>
       </c>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
-        <v>335</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>112</v>
-      </c>
+      <c r="A10" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-    </row>
-    <row r="20" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="15" t="s">
+      <c r="A19" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+    </row>
+    <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="C20" s="16"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="16"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>149</v>
       </c>
       <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>143</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="16"/>
-    </row>
-    <row r="26" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="16"/>
-    </row>
-    <row r="27" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C27" s="16"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
-        <v>356</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-    </row>
-    <row r="32" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="C32" s="16"/>
+      <c r="A31" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+    </row>
+    <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
+  <conditionalFormatting sqref="C11:C19">
+    <cfRule type="cellIs" dxfId="102" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="100" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="98" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C22 C27">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21 C23 C28">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C31">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
@@ -3404,19 +4464,13 @@
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C18 C6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C21 C23</xm:sqref>
+          <xm:sqref>C11:C19 C7 C22 C24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$L$2:$L$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
+          <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3426,11 +4480,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3449,212 +4503,219 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>52</v>
+        <v>404</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>298</v>
+        <v>383</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="19">
+        <v>0</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>320</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>289</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>370</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>332</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="B10" s="20" t="s">
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>328</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="C11" s="19">
-        <v>0</v>
-      </c>
-      <c r="D11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="B12" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>312</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="B15" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>316</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>377</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>330</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>140</v>
+      <c r="B16" s="21" t="s">
+        <v>317</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>318</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A10:D10"/>
   </mergeCells>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="94" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="92" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="90" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
@@ -3664,24 +4725,36 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:D6 C17:D17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C15:D16</xm:sqref>
+          <xm:sqref>C15:D15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:D10</xm:sqref>
+          <xm:sqref>C8:D8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Data Sources'!$C$1:$Z$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:D5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Outputs!$C$1:$Z$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+          <x14:formula1>
+            <xm:f>Lookup!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C13:D14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3691,11 +4764,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3714,18 +4787,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -3736,7 +4809,7 @@
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>5</v>
@@ -3753,7 +4826,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -3762,58 +4835,367 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>334</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="C7" s="28"/>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="C11" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="D11" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>294</v>
-      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C6:D7">
+    <cfRule type="cellIs" dxfId="86" priority="78" operator="equal">
+      <formula>"#466983"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="79" operator="equal">
+      <formula>"green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="80" operator="equal">
+      <formula>"yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+      <formula>"blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+      <formula>"red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+      <formula>"black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+      <formula>"#F0E685"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
+      <formula>"#749B58"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="86" operator="equal">
+      <formula>"#CE3D32"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="87" operator="equal">
+      <formula>"#5050FF"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="76" priority="67" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="71" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="74" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="75" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="76" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="77" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="65" priority="56" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="57" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="59" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="54" priority="45" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="48" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
@@ -3821,10 +5203,119 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Lookup!$M$2:$M$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6:D7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+          <x14:formula1>
+            <xm:f>Lookup!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:D3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -3849,37 +5340,37 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -3889,7 +5380,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3932,7 +5423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
@@ -3949,13 +5440,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3963,7 +5454,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -3974,10 +5465,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3985,7 +5476,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -3996,7 +5487,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -4004,7 +5495,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -4015,13 +5506,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4029,7 +5520,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -4040,10 +5531,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4103,7 +5594,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -4114,18 +5605,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -4136,18 +5627,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -4158,7 +5649,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -4169,7 +5660,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -4180,7 +5671,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
@@ -4191,7 +5682,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
@@ -4202,18 +5693,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -4224,18 +5715,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
@@ -4246,18 +5737,18 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -4268,18 +5759,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>51</v>
@@ -4352,7 +5843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -4369,13 +5860,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4400,12 +5891,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4485,7 +5976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -4502,13 +5993,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4538,87 +6029,87 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B23" s="32"/>
     </row>
@@ -4650,45 +6141,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update documentation of excel template including vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="414">
   <si>
     <t>reportName</t>
   </si>
@@ -1748,9 +1748,6 @@
   </si>
   <si>
     <t>Name of the report file. Remember to include Markdown .md extension. Keep empty to use the default</t>
-  </si>
-  <si>
-    <t>a.md</t>
   </si>
 </sst>
 </file>
@@ -3007,7 +3004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4051,9 +4048,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4124,9 +4121,7 @@
       <c r="B6" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>414</v>
-      </c>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">

</xml_diff>

<commit_message>
Extend explanations of color and fill features of excel template
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="415">
   <si>
     <t>reportName</t>
   </si>
@@ -1741,13 +1741,16 @@
     <t>navy</t>
   </si>
   <si>
-    <t>display color in plots</t>
-  </si>
-  <si>
     <t>If activated: MS Word report will be created additionally to Markdown report</t>
   </si>
   <si>
     <t>Name of the report file. Remember to include Markdown .md extension. Keep empty to use the default</t>
+  </si>
+  <si>
+    <t>display color for lines and points in time profiles and residual plots</t>
+  </si>
+  <si>
+    <t>display color for ranges and histograms in time profiles and residual plots</t>
   </si>
 </sst>
 </file>
@@ -4048,9 +4051,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4119,7 +4122,7 @@
         <v>333</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C6" s="16"/>
     </row>
@@ -4128,7 +4131,7 @@
         <v>133</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>111</v>
@@ -4761,9 +4764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4838,24 +4841,24 @@
         <v>380</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>386</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>388</v>
       </c>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>387</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>388</v>

</xml_diff>

<commit_message>
882 excel template (#956)
* Fixes #855, #870, #873, #882 Excel template accounts for new features

New features include:
- DataSource objects
- Output new parameters
- Workflow title

* Update documentation of excel template including vignette

* Fix methods getting outputs and dataSource names from simulation sets

* Add testing of Excel template features

* Extend explanations of color and fill features of excel template
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15840" tabRatio="914" activeTab="2"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
     <sheet name="Workflow and Tasks" sheetId="13" r:id="rId2"/>
     <sheet name="SimulationSets" sheetId="20" r:id="rId3"/>
-    <sheet name="Outputs_1" sheetId="5" r:id="rId4"/>
-    <sheet name="Userdef PK Parameter" sheetId="15" r:id="rId5"/>
-    <sheet name="PK Parameter" sheetId="14" r:id="rId6"/>
-    <sheet name="PK Conc Single" sheetId="17" r:id="rId7"/>
-    <sheet name="PK Conc Multi" sheetId="18" r:id="rId8"/>
-    <sheet name="PK Fraction" sheetId="19" r:id="rId9"/>
-    <sheet name="SensitivityParameter" sheetId="7" r:id="rId10"/>
-    <sheet name="tpDictionary" sheetId="11" r:id="rId11"/>
-    <sheet name="StudyDesign" sheetId="21" r:id="rId12"/>
-    <sheet name="Lookup" sheetId="16" r:id="rId13"/>
+    <sheet name="Outputs" sheetId="5" r:id="rId4"/>
+    <sheet name="Data Sources" sheetId="22" r:id="rId5"/>
+    <sheet name="Userdef PK Parameter" sheetId="15" r:id="rId6"/>
+    <sheet name="PK Parameter" sheetId="14" r:id="rId7"/>
+    <sheet name="PK Conc Single" sheetId="17" r:id="rId8"/>
+    <sheet name="PK Conc Multi" sheetId="18" r:id="rId9"/>
+    <sheet name="PK Fraction" sheetId="19" r:id="rId10"/>
+    <sheet name="SensitivityParameter" sheetId="7" r:id="rId11"/>
+    <sheet name="tpDictionary" sheetId="11" r:id="rId12"/>
+    <sheet name="StudyDesign" sheetId="21" r:id="rId13"/>
+    <sheet name="Lookup" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="415">
   <si>
     <t>reportName</t>
   </si>
@@ -199,9 +200,6 @@
     <t>Thalf_tLast_tEnd</t>
   </si>
   <si>
-    <t>name of the sheet with the output definitions</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -446,9 +444,6 @@
   </si>
   <si>
     <t>createWordReport</t>
-  </si>
-  <si>
-    <t>If activated: MS Word report will be created additionally to Markdon report</t>
   </si>
   <si>
     <t>simulate: numberOfCores</t>
@@ -1026,12 +1021,6 @@
   </si>
   <si>
     <t>simulationFile</t>
-  </si>
-  <si>
-    <t>Outputs_1</t>
-  </si>
-  <si>
-    <t>observedDataFile</t>
   </si>
   <si>
     <r>
@@ -1423,9 +1412,6 @@
     <t>reportFileName</t>
   </si>
   <si>
-    <t>Name of the report fille; keep empty to use the default</t>
-  </si>
-  <si>
     <t>PlotFormat</t>
   </si>
   <si>
@@ -1578,6 +1564,193 @@
   </si>
   <si>
     <t>Observed data from reference population is plotted in a Simulation Set time profiles of Pediatric and Ratio Comparison workflows</t>
+  </si>
+  <si>
+    <t>dataFile</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>Source1</t>
+  </si>
+  <si>
+    <t>Source2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Displayed data source caption in the report. The caption will be preceeded by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Data source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>groupID</t>
+  </si>
+  <si>
+    <t>identifier for splitting outputs by the combination {displayUnit; groupID}. Each combination becomes then a separate plot</t>
+  </si>
+  <si>
+    <t>reportTitle</t>
+  </si>
+  <si>
+    <t>Title included on top of the report</t>
+  </si>
+  <si>
+    <t>Output1, Output2</t>
+  </si>
+  <si>
+    <t>dataSource</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">name of included data sources defined in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Data Sources </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sheet</t>
+    </r>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>#5050FF</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>#CE3D32</t>
+  </si>
+  <si>
+    <t>#749B58</t>
+  </si>
+  <si>
+    <t>#F0E685</t>
+  </si>
+  <si>
+    <t>#466983</t>
+  </si>
+  <si>
+    <t>#BA6338</t>
+  </si>
+  <si>
+    <t>#5DB1DD</t>
+  </si>
+  <si>
+    <t>#802268</t>
+  </si>
+  <si>
+    <t>#6BD76B</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>magenta</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">name of included outputs defined in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Outputs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet. Separate outputs with a coma to include multiple outputs</t>
+    </r>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>maroon</t>
+  </si>
+  <si>
+    <t>olive</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>navy</t>
+  </si>
+  <si>
+    <t>If activated: MS Word report will be created additionally to Markdown report</t>
+  </si>
+  <si>
+    <t>Name of the report file. Remember to include Markdown .md extension. Keep empty to use the default</t>
+  </si>
+  <si>
+    <t>display color for lines and points in time profiles and residual plots</t>
+  </si>
+  <si>
+    <t>display color for ranges and histograms in time profiles and residual plots</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1782,6 +1955,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1795,8 +1969,744 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="103">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA6338"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5DB1DD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF802268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6BD76B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF800080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF000080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5050FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCE3D32"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF749B58"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF0E685"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF008000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF466983"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000080"/>
+      <color rgb="FF800080"/>
+      <color rgb="FF808000"/>
+      <color rgb="FF800000"/>
+      <color rgb="FF808080"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF008000"/>
+      <color rgb="FF6BD76B"/>
+      <color rgb="FF802268"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2106,26 +3016,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2135,6 +3045,47 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -2147,17 +3098,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -2181,16 +3132,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -2199,18 +3150,18 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2219,13 +3170,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2234,13 +3185,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -2251,30 +3202,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>18</v>
@@ -2285,124 +3236,124 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>94</v>
-      </c>
       <c r="G11" s="9" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +3362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2427,42 +3378,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2473,7 +3424,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -2487,7 +3438,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -2501,7 +3452,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -2515,7 +3466,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -2537,13 +3488,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2560,106 +3511,112 @@
     <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>249</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="L2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
@@ -2668,340 +3625,400 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="L3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+      <c r="M3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+      <c r="M4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="M5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+      <c r="M6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
       </c>
       <c r="J7" t="s">
+        <v>270</v>
+      </c>
+      <c r="L7" t="s">
+        <v>342</v>
+      </c>
+      <c r="M7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" t="s">
+        <v>266</v>
+      </c>
+      <c r="L8" t="s">
+        <v>340</v>
+      </c>
+      <c r="M8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" t="s">
+        <v>271</v>
+      </c>
+      <c r="L9" t="s">
+        <v>341</v>
+      </c>
+      <c r="M9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G10" t="s">
+        <v>211</v>
+      </c>
+      <c r="J10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G11" t="s">
+        <v>212</v>
+      </c>
+      <c r="J11" t="s">
+        <v>237</v>
+      </c>
+      <c r="M11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" t="s">
+        <v>213</v>
+      </c>
+      <c r="J12" t="s">
         <v>272</v>
       </c>
-      <c r="L7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J8" t="s">
-        <v>268</v>
-      </c>
-      <c r="L8" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F9" t="s">
-        <v>202</v>
-      </c>
-      <c r="G9" t="s">
-        <v>212</v>
-      </c>
-      <c r="J9" t="s">
-        <v>273</v>
-      </c>
-      <c r="L9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E10" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" t="s">
-        <v>213</v>
-      </c>
-      <c r="J10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
+      <c r="M12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
         <v>172</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G13" t="s">
         <v>214</v>
-      </c>
-      <c r="J11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E12" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" t="s">
-        <v>215</v>
-      </c>
-      <c r="J12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" t="s">
-        <v>216</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+      <c r="M15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+      <c r="M16" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+      <c r="M18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G22" t="s">
+        <v>222</v>
+      </c>
+      <c r="J22" t="s">
+        <v>276</v>
+      </c>
+      <c r="M22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
         <v>183</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G24" t="s">
         <v>224</v>
       </c>
-      <c r="J22" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E23" t="s">
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
         <v>184</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E24" t="s">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
         <v>185</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E25" t="s">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
         <v>186</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
         <v>187</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G28" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E27" t="s">
+    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
         <v>188</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" t="s">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G29" t="s">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G30" t="s">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="G32" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.2">
@@ -3011,17 +4028,17 @@
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3032,11 +4049,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3055,26 +4072,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>3</v>
@@ -3082,312 +4099,353 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>337</v>
+        <v>381</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>338</v>
+        <v>382</v>
       </c>
       <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>134</v>
+        <v>333</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>112</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>373</v>
+        <v>133</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="C7" s="16"/>
+        <v>411</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>327</v>
+        <v>369</v>
       </c>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
-        <v>335</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>112</v>
-      </c>
+      <c r="A10" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-    </row>
-    <row r="20" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="15" t="s">
+      <c r="A19" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+    </row>
+    <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="C20" s="16"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="16"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>149</v>
       </c>
       <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>143</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="16"/>
-    </row>
-    <row r="26" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="16"/>
-    </row>
-    <row r="27" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C27" s="16"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
-        <v>356</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-    </row>
-    <row r="32" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="C32" s="16"/>
+      <c r="A31" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+    </row>
+    <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
+  <conditionalFormatting sqref="C11:C19">
+    <cfRule type="cellIs" dxfId="102" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="100" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="98" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C22 C27">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21 C23 C28">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:C30">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C31">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
@@ -3404,19 +4462,13 @@
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C18 C6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C21 C23</xm:sqref>
+          <xm:sqref>C11:C19 C7 C22 C24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$L$2:$L$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
+          <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3426,11 +4478,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3449,212 +4501,219 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>52</v>
+        <v>404</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>298</v>
+        <v>383</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="19">
+        <v>0</v>
+      </c>
+      <c r="D9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>320</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>289</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>370</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>332</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="B10" s="20" t="s">
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>328</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="C11" s="19">
-        <v>0</v>
-      </c>
-      <c r="D11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="B12" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>312</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="B15" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>316</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>377</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>330</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>140</v>
+      <c r="B16" s="21" t="s">
+        <v>317</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>318</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A10:D10"/>
   </mergeCells>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="94" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="92" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="90" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
@@ -3664,24 +4723,36 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:D6 C17:D17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
-          <x14:formula1>
-            <xm:f>Lookup!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C15:D16</xm:sqref>
+          <xm:sqref>C15:D15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:D10</xm:sqref>
+          <xm:sqref>C8:D8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Data Sources'!$C$1:$Z$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:D5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Outputs!$C$1:$Z$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+          <x14:formula1>
+            <xm:f>Lookup!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C13:D14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3691,11 +4762,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3714,18 +4785,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -3736,7 +4807,7 @@
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>5</v>
@@ -3753,7 +4824,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -3762,58 +4833,367 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>334</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="C7" s="28"/>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="C11" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="D11" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>294</v>
-      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C6:D7">
+    <cfRule type="cellIs" dxfId="86" priority="78" operator="equal">
+      <formula>"#466983"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="79" operator="equal">
+      <formula>"green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="80" operator="equal">
+      <formula>"yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+      <formula>"blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+      <formula>"red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+      <formula>"black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+      <formula>"#F0E685"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
+      <formula>"#749B58"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="86" operator="equal">
+      <formula>"#CE3D32"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="87" operator="equal">
+      <formula>"#5050FF"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="76" priority="67" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="71" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="74" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="75" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="76" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="77" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="65" priority="56" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="57" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="59" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="54" priority="45" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="48" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
@@ -3821,10 +5201,119 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Lookup!$M$2:$M$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6:D7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+          <x14:formula1>
+            <xm:f>Lookup!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:D3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -3849,37 +5338,37 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -3889,7 +5378,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -3932,7 +5421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
@@ -3949,13 +5438,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3963,7 +5452,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -3974,10 +5463,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3985,7 +5474,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -3996,7 +5485,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -4004,7 +5493,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -4015,13 +5504,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4029,7 +5518,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -4040,10 +5529,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4103,7 +5592,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -4114,18 +5603,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -4136,18 +5625,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -4158,7 +5647,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -4169,7 +5658,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -4180,7 +5669,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
@@ -4191,7 +5680,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
@@ -4202,18 +5691,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -4224,18 +5713,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
@@ -4246,18 +5735,18 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -4268,18 +5757,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>51</v>
@@ -4352,7 +5841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -4369,13 +5858,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4400,12 +5889,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4485,7 +5974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -4502,13 +5991,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4538,87 +6027,87 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B23" s="32"/>
     </row>
@@ -4650,45 +6139,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes #1046 Dictionary in Excel template uses correct column names
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -201,12 +201,6 @@
   </si>
   <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>nonmenColumn</t>
-  </si>
-  <si>
-    <t>nonmemUnit</t>
   </si>
   <si>
     <t>comment</t>
@@ -1751,6 +1745,12 @@
   </si>
   <si>
     <t>display color for ranges and histograms in time profiles and residual plots</t>
+  </si>
+  <si>
+    <t>datasetColumn</t>
+  </si>
+  <si>
+    <t>datasetUnit</t>
   </si>
 </sst>
 </file>
@@ -3016,26 +3016,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3058,13 +3058,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3098,17 +3098,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3121,7 +3121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3130,18 +3132,18 @@
     <col min="7" max="7" width="48.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>53</v>
+        <v>413</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>54</v>
+        <v>414</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -3150,18 +3152,18 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -3170,13 +3172,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3185,13 +3187,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -3202,30 +3204,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>18</v>
@@ -3236,124 +3238,124 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3378,42 +3380,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>357</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3424,7 +3426,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -3438,7 +3440,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -3452,7 +3454,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -3466,7 +3468,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -3513,110 +3515,110 @@
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>247</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
         <v>106</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
@@ -3625,400 +3627,400 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="M6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J14" t="s">
         <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J16" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M16" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
       </c>
       <c r="M17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M18" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
       </c>
       <c r="M20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J21" t="s">
         <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.2">
@@ -4028,17 +4030,17 @@
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4072,26 +4074,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>3</v>
@@ -4099,291 +4101,291 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
     </row>
     <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>159</v>
       </c>
       <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>151</v>
       </c>
       <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
     </row>
     <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C33" s="16"/>
     </row>
@@ -4501,26 +4503,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -4528,71 +4530,71 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>327</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C9" s="19">
         <v>0</v>
@@ -4603,7 +4605,7 @@
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -4611,71 +4613,71 @@
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>315</v>
-      </c>
       <c r="C15" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -4764,9 +4766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4785,18 +4787,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -4807,7 +4809,7 @@
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>5</v>
@@ -4824,7 +4826,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -4835,85 +4837,85 @@
     </row>
     <row r="5" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>386</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>413</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>388</v>
       </c>
       <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C10" s="28"/>
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="D11" s="29" t="s">
         <v>290</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -5238,54 +5240,54 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>304</v>
-      </c>
       <c r="C3" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -5338,37 +5340,37 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -5378,7 +5380,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5438,13 +5440,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5452,7 +5454,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -5463,10 +5465,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5474,7 +5476,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -5485,7 +5487,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -5493,7 +5495,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -5504,13 +5506,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5518,7 +5520,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -5529,10 +5531,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -5592,7 +5594,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -5603,18 +5605,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -5625,18 +5627,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -5647,7 +5649,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -5658,7 +5660,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -5669,7 +5671,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
@@ -5680,7 +5682,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
@@ -5691,18 +5693,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -5713,18 +5715,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
@@ -5735,18 +5737,18 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -5757,18 +5759,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>51</v>
@@ -5858,13 +5860,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5889,12 +5891,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5991,13 +5993,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6027,87 +6029,87 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B23" s="32"/>
     </row>

</xml_diff>

<commit_message>
Fixes #1046 Dictionary in Excel template uses correct column names (#1047)
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -201,12 +201,6 @@
   </si>
   <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>nonmenColumn</t>
-  </si>
-  <si>
-    <t>nonmemUnit</t>
   </si>
   <si>
     <t>comment</t>
@@ -1751,6 +1745,12 @@
   </si>
   <si>
     <t>display color for ranges and histograms in time profiles and residual plots</t>
+  </si>
+  <si>
+    <t>datasetColumn</t>
+  </si>
+  <si>
+    <t>datasetUnit</t>
   </si>
 </sst>
 </file>
@@ -3016,26 +3016,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3058,13 +3058,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3098,17 +3098,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3121,7 +3121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3130,18 +3132,18 @@
     <col min="7" max="7" width="48.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>53</v>
+        <v>413</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>54</v>
+        <v>414</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -3150,18 +3152,18 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -3170,13 +3172,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -3185,13 +3187,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>18</v>
@@ -3202,30 +3204,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>18</v>
@@ -3236,124 +3238,124 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3378,42 +3380,42 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>357</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3424,7 +3426,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
@@ -3438,7 +3440,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D5" s="9">
         <v>2.5</v>
@@ -3452,7 +3454,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -3466,7 +3468,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D7" s="9">
         <v>14</v>
@@ -3513,110 +3515,110 @@
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>247</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
         <v>106</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
@@ -3625,400 +3627,400 @@
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="M6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J14" t="s">
         <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J16" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M16" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
       </c>
       <c r="M17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M18" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
       </c>
       <c r="M20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J21" t="s">
         <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.2">
@@ -4028,17 +4030,17 @@
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4072,26 +4074,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>3</v>
@@ -4099,291 +4101,291 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
     </row>
     <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>159</v>
       </c>
       <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>151</v>
       </c>
       <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
     </row>
     <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C33" s="16"/>
     </row>
@@ -4501,26 +4503,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -4528,71 +4530,71 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>327</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C9" s="19">
         <v>0</v>
@@ -4603,7 +4605,7 @@
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="36"/>
@@ -4611,71 +4613,71 @@
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>315</v>
-      </c>
       <c r="C15" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -4764,9 +4766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4785,18 +4787,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -4807,7 +4809,7 @@
     </row>
     <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>5</v>
@@ -4824,7 +4826,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>12</v>
@@ -4835,85 +4837,85 @@
     </row>
     <row r="5" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>386</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>413</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>388</v>
       </c>
       <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C10" s="28"/>
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="D11" s="29" t="s">
         <v>290</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -5238,54 +5240,54 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>304</v>
-      </c>
       <c r="C3" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -5338,37 +5340,37 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -5378,7 +5380,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -5438,13 +5440,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5452,7 +5454,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -5463,10 +5465,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5474,7 +5476,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -5485,7 +5487,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -5493,7 +5495,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -5504,13 +5506,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5518,7 +5520,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -5529,10 +5531,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -5592,7 +5594,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -5603,18 +5605,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -5625,18 +5627,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -5647,7 +5649,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -5658,7 +5660,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -5669,7 +5671,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
@@ -5680,7 +5682,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
@@ -5691,18 +5693,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -5713,18 +5715,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
@@ -5735,18 +5737,18 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -5757,18 +5759,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>51</v>
@@ -5858,13 +5860,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5889,12 +5891,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5991,13 +5993,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6027,87 +6029,87 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B23" s="32"/>
     </row>

</xml_diff>

<commit_message>
Fixes #1131 excel template include mass balance settings
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E628B-3D09-427D-86C7-71105F3B5A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="12885" tabRatio="914" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -28,21 +29,11 @@
     <sheet name="Lookup" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="418">
   <si>
     <t>reportName</t>
   </si>
@@ -1752,11 +1743,20 @@
   <si>
     <t>datasetUnit</t>
   </si>
+  <si>
+    <t>All settings below are relevant for MEANMODEL workflows only</t>
+  </si>
+  <si>
+    <t>massBalanceFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path to the mass balance settings (json) RELATIVE to workflow.R, e.g. mass-balance-settings.json or Models/mass-balance-settings.json </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1889,7 +1889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1908,7 +1908,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1919,7 +1919,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1941,7 +1940,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1950,12 +1949,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1969,81 +1963,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFBA6338"/>
+          <bgColor rgb="FFCE3D32"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF5DB1DD"/>
+          <bgColor rgb="FF749B58"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF802268"/>
+          <bgColor rgb="FFF0E685"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF6BD76B"/>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF0000FF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF808080"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF800000"/>
+          <bgColor rgb="FF008000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF808000"/>
+          <bgColor rgb="FF466983"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000080"/>
+          <bgColor rgb="FF5050FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2121,503 +2108,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF000080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA6338"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5DB1DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF802268"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6BD76B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA6338"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5DB1DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF802268"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6BD76B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA6338"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5DB1DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF802268"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6BD76B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA6338"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5DB1DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF802268"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6BD76B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA6338"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5DB1DD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF802268"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6BD76B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF800080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF000080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5050FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCE3D32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF749B58"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF0E685"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF008000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF466983"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2719,9 +2209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2759,9 +2249,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2796,7 +2286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2831,7 +2321,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3004,7 +2494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3045,7 +2535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3063,7 +2553,7 @@
       <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3071,13 +2561,11 @@
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3086,7 +2574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3118,10 +2606,10 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -3365,7 +2853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3491,7 +2979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3591,7 +3079,7 @@
       <c r="L2" t="s">
         <v>333</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" t="s">
         <v>386</v>
       </c>
     </row>
@@ -4050,7 +3538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4067,327 +3555,327 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>380</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="28" t="s">
         <v>330</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
     </row>
     <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="16"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="28" t="s">
         <v>349</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
     </row>
     <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="C33" s="16"/>
+      <c r="C33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4395,78 +3883,78 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A32:C32"/>
   </mergeCells>
-  <conditionalFormatting sqref="C11:C19">
-    <cfRule type="cellIs" dxfId="102" priority="7" operator="equal">
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="100" priority="5" operator="equal">
+  <conditionalFormatting sqref="C11:C19">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="98" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="96" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21 C23 C28">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21 C23 C28" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C31">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C31" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" sqref="C8" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>Lookup!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>Lookup!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>C11:C19 C7 C22 C24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>Lookup!$L$2:$L$9</xm:f>
           </x14:formula1>
@@ -4479,12 +3967,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4495,229 +3983,222 @@
     <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:4" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>381</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
         <v>382</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:4" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>343</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>416</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="94" priority="7" operator="equal">
+  <conditionalFormatting sqref="C13:D14">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="92" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="90" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
     </dataValidation>
   </dataValidations>
@@ -4726,31 +4207,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>C15:D15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C8:D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>'Data Sources'!$C$1:$Z$1</xm:f>
           </x14:formula1>
           <xm:sqref>C5:D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
           <x14:formula1>
             <xm:f>Outputs!$C$1:$Z$1</xm:f>
           </x14:formula1>
           <xm:sqref>C4:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0200-000005000000}">
           <x14:formula1>
             <xm:f>Lookup!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -4763,7 +4244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4779,425 +4260,211 @@
     <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:4" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>344</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>384</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+    </row>
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>385</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+    </row>
+    <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="C10" s="28"/>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="18" t="s">
         <v>290</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:D7">
-    <cfRule type="cellIs" dxfId="86" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+      <formula>"navy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+      <formula>"olive"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>"maroon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>"gray"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>"cyan"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>"magenta"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+      <formula>"#6BD76B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>"#802268"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"#5DB1DD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"#BA6338"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="87" operator="equal">
+      <formula>"#5050FF"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="78" operator="equal">
       <formula>"#466983"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="79" operator="equal">
       <formula>"green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="80" operator="equal">
       <formula>"yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="81" operator="equal">
       <formula>"blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="82" operator="equal">
       <formula>"red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="83" operator="equal">
       <formula>"black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="84" operator="equal">
       <formula>"#F0E685"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="85" operator="equal">
       <formula>"#749B58"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="86" operator="equal">
       <formula>"#CE3D32"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="87" operator="equal">
-      <formula>"#5050FF"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="76" priority="67" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="71" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="74" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="75" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="76" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="77" operator="equal">
-      <formula>"#BA6338"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="65" priority="56" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="57" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="58" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="59" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="60" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
-      <formula>"#BA6338"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="54" priority="45" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="48" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="52" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
-      <formula>"#BA6338"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
-      <formula>"#BA6338"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
-      <formula>"#BA6338"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
-      <formula>"#BA6338"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
-      <formula>"navy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
-      <formula>"purple"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>"olive"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>"maroon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
-      <formula>"gray"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"cyan"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
-      <formula>"magenta"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
-      <formula>"#6BD76B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
-      <formula>"#802268"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
-      <formula>"#5DB1DD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
-      <formula>"#BA6338"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
     </dataValidation>
   </dataValidations>
@@ -5206,7 +4473,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>Lookup!$M$2:$M$22</xm:f>
           </x14:formula1>
@@ -5219,7 +4486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5233,68 +4500,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>373</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>376</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only alphanumeric values allowed" sqref="C1:D1" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
     </dataValidation>
   </dataValidations>
@@ -5303,7 +4570,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>Lookup!$K$2:$K$3</xm:f>
           </x14:formula1>
@@ -5316,7 +4583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5399,10 +4666,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100 F2:G100 I2:I100 K2:K100">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D100 F2:G100 I2:I100 K2:K100" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E100 H2:H100">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E100 H2:H100" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -5411,7 +4678,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0500-000002000000}">
           <x14:formula1>
             <xm:f>Lookup!$J$2:$J$22</xm:f>
           </x14:formula1>
@@ -5424,7 +4691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5786,7 +5053,7 @@
       <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5797,7 +5064,7 @@
       <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5807,31 +5074,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3 C5 C15:C18 C21:C22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>C31 C4 C10:C11 C19:C20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0600-000002000000}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>C6:C9 C23:C30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0600-000003000000}">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>C12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0600-000004000000}">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
@@ -5844,7 +5111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5865,7 +5132,7 @@
       <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>159</v>
       </c>
     </row>
@@ -5940,31 +5207,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0700-000000000000}">
           <x14:formula1>
             <xm:f>Lookup!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0700-000001000000}">
           <x14:formula1>
             <xm:f>Lookup!$H$2:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0700-000002000000}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>
           <xm:sqref>B6:B9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0700-000003000000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4 B10:B11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0700-000004000000}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
@@ -5977,7 +5244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5998,7 +5265,7 @@
       <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>159</v>
       </c>
     </row>
@@ -6077,41 +5344,40 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B23" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -6119,19 +5385,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>Lookup!$E$2:$E$29</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B3 B7:B10 B13:B14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0800-000001000000}">
           <x14:formula1>
             <xm:f>Lookup!$F$2:$F$9</xm:f>
           </x14:formula1>
           <xm:sqref>B23 B4:B6 B11:B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid value. Please select from the list" xr:uid="{00000000-0002-0000-0800-000002000000}">
           <x14:formula1>
             <xm:f>Lookup!$G$2:$G$37</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Fixes #1244 dictionaries use consistent comment
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E628B-3D09-427D-86C7-71105F3B5A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6244981-9F1B-4280-9D87-79CDA783064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -1504,9 +1504,6 @@
     <t>FEMALE</t>
   </si>
   <si>
-    <t>Make sure 1=male 2= female</t>
-  </si>
-  <si>
     <t>ALL</t>
   </si>
   <si>
@@ -1751,6 +1748,9 @@
   </si>
   <si>
     <t xml:space="preserve">Path to the mass balance settings (json) RELATIVE to workflow.R, e.g. mass-balance-settings.json or Models/mass-balance-settings.json </t>
+  </si>
+  <si>
+    <t>Make sure male="MALE" and female="FEMALE"</t>
   </si>
 </sst>
 </file>
@@ -1967,6 +1967,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF5050FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFCE3D32"/>
         </patternFill>
       </fill>
@@ -2024,13 +2031,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF466983"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5050FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2609,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2628,10 +2628,10 @@
         <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>414</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -2826,7 +2826,7 @@
         <v>91</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>360</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3039,7 +3039,7 @@
         <v>332</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3080,7 +3080,7 @@
         <v>333</v>
       </c>
       <c r="M2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3121,7 +3121,7 @@
         <v>334</v>
       </c>
       <c r="M3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3147,7 +3147,7 @@
         <v>335</v>
       </c>
       <c r="M4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3170,7 +3170,7 @@
         <v>336</v>
       </c>
       <c r="M5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -3190,7 +3190,7 @@
         <v>337</v>
       </c>
       <c r="M6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -3210,7 +3210,7 @@
         <v>340</v>
       </c>
       <c r="M7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3230,7 +3230,7 @@
         <v>338</v>
       </c>
       <c r="M8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3250,7 +3250,7 @@
         <v>339</v>
       </c>
       <c r="M9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -3264,7 +3264,7 @@
         <v>200</v>
       </c>
       <c r="M10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3278,7 +3278,7 @@
         <v>235</v>
       </c>
       <c r="M11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3292,7 +3292,7 @@
         <v>270</v>
       </c>
       <c r="M12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -3306,7 +3306,7 @@
         <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -3320,7 +3320,7 @@
         <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -3334,7 +3334,7 @@
         <v>271</v>
       </c>
       <c r="M15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3348,7 +3348,7 @@
         <v>272</v>
       </c>
       <c r="M16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.2">
@@ -3362,7 +3362,7 @@
         <v>25</v>
       </c>
       <c r="M17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.2">
@@ -3376,7 +3376,7 @@
         <v>273</v>
       </c>
       <c r="M18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.2">
@@ -3390,7 +3390,7 @@
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.2">
@@ -3404,7 +3404,7 @@
         <v>29</v>
       </c>
       <c r="M20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
         <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.2">
@@ -3432,7 +3432,7 @@
         <v>274</v>
       </c>
       <c r="M22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.2">
@@ -3570,7 +3570,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>105</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>380</v>
       </c>
       <c r="C5" s="15"/>
     </row>
@@ -3612,7 +3612,7 @@
         <v>331</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -3621,7 +3621,7 @@
         <v>131</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>109</v>
@@ -3629,10 +3629,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>366</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>367</v>
       </c>
       <c r="C8" s="15"/>
     </row>
@@ -3970,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -4018,21 +4018,21 @@
         <v>4</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>382</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
@@ -4040,13 +4040,13 @@
         <v>285</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4120,7 +4120,7 @@
         <v>310</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>110</v>
@@ -4134,7 +4134,7 @@
         <v>324</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>110</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>415</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -4318,32 +4318,32 @@
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>377</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>385</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
@@ -4351,13 +4351,13 @@
         <v>285</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -4371,15 +4371,15 @@
         <v>328</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>368</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>369</v>
       </c>
       <c r="C10" s="21"/>
     </row>
@@ -4432,35 +4432,35 @@
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"#BA6338"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="87" operator="equal">
-      <formula>"#5050FF"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="78" operator="equal">
       <formula>"#466983"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="79" operator="equal">
       <formula>"green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="80" operator="equal">
       <formula>"yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="81" operator="equal">
       <formula>"blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="82" operator="equal">
       <formula>"red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="83" operator="equal">
       <formula>"black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="84" operator="equal">
       <formula>"#F0E685"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="85" operator="equal">
       <formula>"#749B58"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="86" operator="equal">
       <formula>"#CE3D32"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="equal">
+      <formula>"#5050FF"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4507,15 +4507,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>374</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>295</v>
@@ -4551,10 +4551,10 @@
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>

</xml_diff>

<commit_message>
Fixes #1244 dictionaries use consistent comment (#1245)
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E628B-3D09-427D-86C7-71105F3B5A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6244981-9F1B-4280-9D87-79CDA783064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -1504,9 +1504,6 @@
     <t>FEMALE</t>
   </si>
   <si>
-    <t>Make sure 1=male 2= female</t>
-  </si>
-  <si>
     <t>ALL</t>
   </si>
   <si>
@@ -1751,6 +1748,9 @@
   </si>
   <si>
     <t xml:space="preserve">Path to the mass balance settings (json) RELATIVE to workflow.R, e.g. mass-balance-settings.json or Models/mass-balance-settings.json </t>
+  </si>
+  <si>
+    <t>Make sure male="MALE" and female="FEMALE"</t>
   </si>
 </sst>
 </file>
@@ -1967,6 +1967,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF5050FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFCE3D32"/>
         </patternFill>
       </fill>
@@ -2024,13 +2031,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF466983"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5050FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2609,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2628,10 +2628,10 @@
         <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>414</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -2826,7 +2826,7 @@
         <v>91</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>360</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3039,7 +3039,7 @@
         <v>332</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3080,7 +3080,7 @@
         <v>333</v>
       </c>
       <c r="M2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3121,7 +3121,7 @@
         <v>334</v>
       </c>
       <c r="M3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3147,7 +3147,7 @@
         <v>335</v>
       </c>
       <c r="M4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3170,7 +3170,7 @@
         <v>336</v>
       </c>
       <c r="M5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -3190,7 +3190,7 @@
         <v>337</v>
       </c>
       <c r="M6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -3210,7 +3210,7 @@
         <v>340</v>
       </c>
       <c r="M7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3230,7 +3230,7 @@
         <v>338</v>
       </c>
       <c r="M8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3250,7 +3250,7 @@
         <v>339</v>
       </c>
       <c r="M9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -3264,7 +3264,7 @@
         <v>200</v>
       </c>
       <c r="M10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3278,7 +3278,7 @@
         <v>235</v>
       </c>
       <c r="M11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3292,7 +3292,7 @@
         <v>270</v>
       </c>
       <c r="M12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -3306,7 +3306,7 @@
         <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -3320,7 +3320,7 @@
         <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -3334,7 +3334,7 @@
         <v>271</v>
       </c>
       <c r="M15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3348,7 +3348,7 @@
         <v>272</v>
       </c>
       <c r="M16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.2">
@@ -3362,7 +3362,7 @@
         <v>25</v>
       </c>
       <c r="M17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.2">
@@ -3376,7 +3376,7 @@
         <v>273</v>
       </c>
       <c r="M18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.2">
@@ -3390,7 +3390,7 @@
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.2">
@@ -3404,7 +3404,7 @@
         <v>29</v>
       </c>
       <c r="M20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
         <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.2">
@@ -3432,7 +3432,7 @@
         <v>274</v>
       </c>
       <c r="M22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.2">
@@ -3570,7 +3570,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>105</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>380</v>
       </c>
       <c r="C5" s="15"/>
     </row>
@@ -3612,7 +3612,7 @@
         <v>331</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -3621,7 +3621,7 @@
         <v>131</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>109</v>
@@ -3629,10 +3629,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>366</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>367</v>
       </c>
       <c r="C8" s="15"/>
     </row>
@@ -3970,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -4018,21 +4018,21 @@
         <v>4</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>382</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
@@ -4040,13 +4040,13 @@
         <v>285</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4120,7 +4120,7 @@
         <v>310</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>110</v>
@@ -4134,7 +4134,7 @@
         <v>324</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>110</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>415</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -4318,32 +4318,32 @@
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>377</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>385</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
@@ -4351,13 +4351,13 @@
         <v>285</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -4371,15 +4371,15 @@
         <v>328</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>368</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>369</v>
       </c>
       <c r="C10" s="21"/>
     </row>
@@ -4432,35 +4432,35 @@
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"#BA6338"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="87" operator="equal">
-      <formula>"#5050FF"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="78" operator="equal">
       <formula>"#466983"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="79" operator="equal">
       <formula>"green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="80" operator="equal">
       <formula>"yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="81" operator="equal">
       <formula>"blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="82" operator="equal">
       <formula>"red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="83" operator="equal">
       <formula>"black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="84" operator="equal">
       <formula>"#F0E685"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="85" operator="equal">
       <formula>"#749B58"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="86" operator="equal">
       <formula>"#CE3D32"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="equal">
+      <formula>"#5050FF"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4507,15 +4507,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>374</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>295</v>
@@ -4551,10 +4551,10 @@
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>

</xml_diff>

<commit_message>
Fixes #1046 use 2 template dictionaries with and without LLOQ
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre Chelle\Documents\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6244981-9F1B-4280-9D87-79CDA783064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837E7BE3-612B-4C2C-885D-28F9B403B082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="914" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -25,15 +25,16 @@
     <sheet name="PK Fraction" sheetId="19" r:id="rId10"/>
     <sheet name="SensitivityParameter" sheetId="7" r:id="rId11"/>
     <sheet name="tpDictionary" sheetId="11" r:id="rId12"/>
-    <sheet name="StudyDesign" sheetId="21" r:id="rId13"/>
-    <sheet name="Lookup" sheetId="16" r:id="rId14"/>
+    <sheet name="tpDictionaryLoq" sheetId="23" r:id="rId13"/>
+    <sheet name="StudyDesign" sheetId="21" r:id="rId14"/>
+    <sheet name="Lookup" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="418">
   <si>
     <t>reportName</t>
   </si>
@@ -1889,7 +1890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1959,6 +1960,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2499,12 +2502,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>93</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>94</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>95</v>
       </c>
@@ -2540,13 +2543,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -2557,12 +2560,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2579,22 +2582,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -2607,20 +2610,20 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="48.125" customWidth="1"/>
+    <col min="7" max="7" width="48.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>318</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -2658,7 +2661,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
@@ -2673,7 +2676,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
@@ -2690,7 +2693,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
@@ -2724,7 +2727,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -2745,7 +2748,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>75</v>
       </c>
@@ -2766,7 +2769,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>80</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>85</v>
       </c>
@@ -2808,7 +2811,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>89</v>
       </c>
@@ -2827,23 +2830,6 @@
       </c>
       <c r="G11" s="9" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2853,20 +2839,270 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05B762A-0A3E-4AE3-9238-C14EE5C34AFE}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.4140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="19.08203125" customWidth="1"/>
     <col min="4" max="4" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>79</v>
       </c>
@@ -2880,7 +3116,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
@@ -2892,7 +3128,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>354</v>
       </c>
@@ -2906,7 +3142,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>20</v>
       </c>
@@ -2920,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>20</v>
       </c>
@@ -2934,7 +3170,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>40</v>
       </c>
@@ -2948,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>40</v>
       </c>
@@ -2962,7 +3198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>60</v>
       </c>
@@ -2978,7 +3214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
@@ -2987,21 +3223,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>103</v>
       </c>
@@ -3042,7 +3278,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -3083,7 +3319,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -3124,7 +3360,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>107</v>
       </c>
@@ -3150,7 +3386,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>162</v>
       </c>
@@ -3173,7 +3409,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>163</v>
       </c>
@@ -3193,7 +3429,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>164</v>
       </c>
@@ -3213,7 +3449,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>165</v>
       </c>
@@ -3233,7 +3469,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>166</v>
       </c>
@@ -3253,7 +3489,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>167</v>
       </c>
@@ -3267,7 +3503,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>168</v>
       </c>
@@ -3281,7 +3517,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>169</v>
       </c>
@@ -3295,7 +3531,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>170</v>
       </c>
@@ -3309,7 +3545,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>171</v>
       </c>
@@ -3323,7 +3559,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>172</v>
       </c>
@@ -3337,7 +3573,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>173</v>
       </c>
@@ -3351,7 +3587,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>174</v>
       </c>
@@ -3365,7 +3601,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>175</v>
       </c>
@@ -3379,7 +3615,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>176</v>
       </c>
@@ -3393,7 +3629,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>177</v>
       </c>
@@ -3407,7 +3643,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>178</v>
       </c>
@@ -3421,7 +3657,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>179</v>
       </c>
@@ -3435,7 +3671,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>180</v>
       </c>
@@ -3443,7 +3679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>181</v>
       </c>
@@ -3451,7 +3687,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>182</v>
       </c>
@@ -3459,7 +3695,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>183</v>
       </c>
@@ -3467,7 +3703,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>184</v>
       </c>
@@ -3475,7 +3711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>185</v>
       </c>
@@ -3483,7 +3719,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>186</v>
       </c>
@@ -3491,42 +3727,42 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>234</v>
       </c>
@@ -3546,7 +3782,7 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="100.25" customWidth="1"/>
@@ -3554,7 +3790,7 @@
     <col min="6" max="6" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3565,7 +3801,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="38" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -3576,7 +3812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
@@ -3587,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>129</v>
       </c>
@@ -3598,7 +3834,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>378</v>
       </c>
@@ -3607,7 +3843,7 @@
       </c>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>331</v>
       </c>
@@ -3616,7 +3852,7 @@
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>131</v>
       </c>
@@ -3627,7 +3863,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>365</v>
       </c>
@@ -3636,7 +3872,7 @@
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>320</v>
       </c>
@@ -3645,14 +3881,14 @@
       </c>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>329</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>111</v>
       </c>
@@ -3663,7 +3899,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>113</v>
       </c>
@@ -3674,7 +3910,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>115</v>
       </c>
@@ -3685,7 +3921,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>117</v>
       </c>
@@ -3696,7 +3932,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>119</v>
       </c>
@@ -3707,7 +3943,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>121</v>
       </c>
@@ -3718,7 +3954,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>123</v>
       </c>
@@ -3729,7 +3965,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>124</v>
       </c>
@@ -3740,7 +3976,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>125</v>
       </c>
@@ -3751,14 +3987,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>330</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
     </row>
-    <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>132</v>
       </c>
@@ -3767,7 +4003,7 @@
       </c>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>133</v>
       </c>
@@ -3778,7 +4014,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>137</v>
       </c>
@@ -3787,7 +4023,7 @@
       </c>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>138</v>
       </c>
@@ -3796,7 +4032,7 @@
       </c>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>140</v>
       </c>
@@ -3807,7 +4043,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>141</v>
       </c>
@@ -3816,7 +4052,7 @@
       </c>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="38" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>155</v>
       </c>
@@ -3825,7 +4061,7 @@
       </c>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>147</v>
       </c>
@@ -3834,7 +4070,7 @@
       </c>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>148</v>
       </c>
@@ -3843,7 +4079,7 @@
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>151</v>
       </c>
@@ -3852,7 +4088,7 @@
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>153</v>
       </c>
@@ -3861,14 +4097,14 @@
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>349</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
     </row>
-    <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>350</v>
       </c>
@@ -3975,15 +4211,15 @@
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="42.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.75" customWidth="1"/>
     <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -3997,7 +4233,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>291</v>
       </c>
@@ -4005,7 +4241,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>293</v>
       </c>
@@ -4013,7 +4249,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
@@ -4027,7 +4263,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>381</v>
       </c>
@@ -4035,7 +4271,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>285</v>
       </c>
@@ -4049,7 +4285,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>286</v>
       </c>
@@ -4063,7 +4299,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>303</v>
       </c>
@@ -4077,7 +4313,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>322</v>
       </c>
@@ -4091,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>305</v>
       </c>
@@ -4099,7 +4335,7 @@
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>306</v>
       </c>
@@ -4107,7 +4343,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>308</v>
       </c>
@@ -4115,7 +4351,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>310</v>
       </c>
@@ -4129,7 +4365,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="18" customFormat="1" ht="38" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -4143,7 +4379,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>311</v>
       </c>
@@ -4157,7 +4393,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="18" customFormat="1" ht="89" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>312</v>
       </c>
@@ -4168,7 +4404,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>414</v>
       </c>
@@ -4176,7 +4412,7 @@
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>415</v>
       </c>
@@ -4252,15 +4488,15 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.75" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.58203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -4274,7 +4510,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>283</v>
       </c>
@@ -4288,7 +4524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>284</v>
       </c>
@@ -4302,7 +4538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>11</v>
       </c>
@@ -4316,7 +4552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>376</v>
       </c>
@@ -4324,7 +4560,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>383</v>
       </c>
@@ -4335,7 +4571,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>384</v>
       </c>
@@ -4346,7 +4582,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="18" customFormat="1" ht="140" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>285</v>
       </c>
@@ -4360,7 +4596,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>286</v>
       </c>
@@ -4374,7 +4610,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>367</v>
       </c>
@@ -4383,7 +4619,7 @@
       </c>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>287</v>
       </c>
@@ -4489,17 +4725,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -4513,7 +4751,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>371</v>
       </c>
@@ -4523,7 +4761,7 @@
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>300</v>
       </c>
@@ -4537,7 +4775,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>296</v>
       </c>
@@ -4549,7 +4787,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="63.5" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>372</v>
       </c>
@@ -4591,21 +4829,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.58203125" customWidth="1"/>
+    <col min="2" max="2" width="27.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -4642,7 +4880,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4653,7 +4891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4699,13 +4937,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -4716,7 +4954,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -4727,7 +4965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4738,7 +4976,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -4749,7 +4987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -4760,7 +4998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
@@ -4771,7 +5009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>235</v>
       </c>
@@ -4782,7 +5020,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -4793,7 +5031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -4804,7 +5042,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -4815,7 +5053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -4826,7 +5064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -4837,7 +5075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -4848,7 +5086,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4859,7 +5097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>247</v>
       </c>
@@ -4870,7 +5108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>248</v>
       </c>
@@ -4881,7 +5119,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>249</v>
       </c>
@@ -4892,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>250</v>
       </c>
@@ -4903,7 +5141,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>251</v>
       </c>
@@ -4914,7 +5152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>252</v>
       </c>
@@ -4925,7 +5163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>253</v>
       </c>
@@ -4936,7 +5174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>254</v>
       </c>
@@ -4947,7 +5185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>255</v>
       </c>
@@ -4958,7 +5196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>256</v>
       </c>
@@ -4969,7 +5207,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>257</v>
       </c>
@@ -4980,7 +5218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>258</v>
       </c>
@@ -4991,7 +5229,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>259</v>
       </c>
@@ -5002,7 +5240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>260</v>
       </c>
@@ -5013,7 +5251,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>261</v>
       </c>
@@ -5024,7 +5262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>262</v>
       </c>
@@ -5035,7 +5273,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="11" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>263</v>
       </c>
@@ -5046,7 +5284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -5057,7 +5295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -5119,13 +5357,13 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -5136,67 +5374,67 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -5252,13 +5490,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -5269,112 +5507,112 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>263</v>
       </c>

</xml_diff>

<commit_message>
Fixes #1046 use 2 template dictionaries with and without LLOQ (#1273)
</commit_message>
<xml_diff>
--- a/inst/extdata/WorkflowInput.xlsx
+++ b/inst/extdata/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre Chelle\Documents\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6244981-9F1B-4280-9D87-79CDA783064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837E7BE3-612B-4C2C-885D-28F9B403B082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="914" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -25,15 +25,16 @@
     <sheet name="PK Fraction" sheetId="19" r:id="rId10"/>
     <sheet name="SensitivityParameter" sheetId="7" r:id="rId11"/>
     <sheet name="tpDictionary" sheetId="11" r:id="rId12"/>
-    <sheet name="StudyDesign" sheetId="21" r:id="rId13"/>
-    <sheet name="Lookup" sheetId="16" r:id="rId14"/>
+    <sheet name="tpDictionaryLoq" sheetId="23" r:id="rId13"/>
+    <sheet name="StudyDesign" sheetId="21" r:id="rId14"/>
+    <sheet name="Lookup" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="418">
   <si>
     <t>reportName</t>
   </si>
@@ -1889,7 +1890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1959,6 +1960,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2499,12 +2502,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>93</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>94</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>95</v>
       </c>
@@ -2540,13 +2543,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -2557,12 +2560,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2579,22 +2582,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -2607,20 +2610,20 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="48.125" customWidth="1"/>
+    <col min="7" max="7" width="48.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>318</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -2658,7 +2661,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
@@ -2673,7 +2676,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
@@ -2690,7 +2693,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
@@ -2724,7 +2727,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -2745,7 +2748,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>75</v>
       </c>
@@ -2766,7 +2769,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>80</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>85</v>
       </c>
@@ -2808,7 +2811,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>89</v>
       </c>
@@ -2827,23 +2830,6 @@
       </c>
       <c r="G11" s="9" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2853,20 +2839,270 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05B762A-0A3E-4AE3-9238-C14EE5C34AFE}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.4140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="19.08203125" customWidth="1"/>
     <col min="4" max="4" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>79</v>
       </c>
@@ -2880,7 +3116,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
@@ -2892,7 +3128,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>354</v>
       </c>
@@ -2906,7 +3142,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>20</v>
       </c>
@@ -2920,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>20</v>
       </c>
@@ -2934,7 +3170,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>40</v>
       </c>
@@ -2948,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>40</v>
       </c>
@@ -2962,7 +3198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>60</v>
       </c>
@@ -2978,7 +3214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
@@ -2987,21 +3223,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>103</v>
       </c>
@@ -3042,7 +3278,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -3083,7 +3319,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -3124,7 +3360,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>107</v>
       </c>
@@ -3150,7 +3386,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>162</v>
       </c>
@@ -3173,7 +3409,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>163</v>
       </c>
@@ -3193,7 +3429,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>164</v>
       </c>
@@ -3213,7 +3449,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>165</v>
       </c>
@@ -3233,7 +3469,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>166</v>
       </c>
@@ -3253,7 +3489,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>167</v>
       </c>
@@ -3267,7 +3503,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>168</v>
       </c>
@@ -3281,7 +3517,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>169</v>
       </c>
@@ -3295,7 +3531,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>170</v>
       </c>
@@ -3309,7 +3545,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>171</v>
       </c>
@@ -3323,7 +3559,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>172</v>
       </c>
@@ -3337,7 +3573,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>173</v>
       </c>
@@ -3351,7 +3587,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>174</v>
       </c>
@@ -3365,7 +3601,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>175</v>
       </c>
@@ -3379,7 +3615,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>176</v>
       </c>
@@ -3393,7 +3629,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>177</v>
       </c>
@@ -3407,7 +3643,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>178</v>
       </c>
@@ -3421,7 +3657,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>179</v>
       </c>
@@ -3435,7 +3671,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>180</v>
       </c>
@@ -3443,7 +3679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>181</v>
       </c>
@@ -3451,7 +3687,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>182</v>
       </c>
@@ -3459,7 +3695,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>183</v>
       </c>
@@ -3467,7 +3703,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>184</v>
       </c>
@@ -3475,7 +3711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>185</v>
       </c>
@@ -3483,7 +3719,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>186</v>
       </c>
@@ -3491,42 +3727,42 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>234</v>
       </c>
@@ -3546,7 +3782,7 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="100.25" customWidth="1"/>
@@ -3554,7 +3790,7 @@
     <col min="6" max="6" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3565,7 +3801,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="38" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -3576,7 +3812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
@@ -3587,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>129</v>
       </c>
@@ -3598,7 +3834,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>378</v>
       </c>
@@ -3607,7 +3843,7 @@
       </c>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>331</v>
       </c>
@@ -3616,7 +3852,7 @@
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>131</v>
       </c>
@@ -3627,7 +3863,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>365</v>
       </c>
@@ -3636,7 +3872,7 @@
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>320</v>
       </c>
@@ -3645,14 +3881,14 @@
       </c>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>329</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>111</v>
       </c>
@@ -3663,7 +3899,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>113</v>
       </c>
@@ -3674,7 +3910,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>115</v>
       </c>
@@ -3685,7 +3921,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>117</v>
       </c>
@@ -3696,7 +3932,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>119</v>
       </c>
@@ -3707,7 +3943,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>121</v>
       </c>
@@ -3718,7 +3954,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>123</v>
       </c>
@@ -3729,7 +3965,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>124</v>
       </c>
@@ -3740,7 +3976,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>125</v>
       </c>
@@ -3751,14 +3987,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>330</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
     </row>
-    <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>132</v>
       </c>
@@ -3767,7 +4003,7 @@
       </c>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>133</v>
       </c>
@@ -3778,7 +4014,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>137</v>
       </c>
@@ -3787,7 +4023,7 @@
       </c>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>138</v>
       </c>
@@ -3796,7 +4032,7 @@
       </c>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>140</v>
       </c>
@@ -3807,7 +4043,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>141</v>
       </c>
@@ -3816,7 +4052,7 @@
       </c>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="38" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>155</v>
       </c>
@@ -3825,7 +4061,7 @@
       </c>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>147</v>
       </c>
@@ -3834,7 +4070,7 @@
       </c>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>148</v>
       </c>
@@ -3843,7 +4079,7 @@
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>151</v>
       </c>
@@ -3852,7 +4088,7 @@
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>153</v>
       </c>
@@ -3861,14 +4097,14 @@
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>349</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
     </row>
-    <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>350</v>
       </c>
@@ -3975,15 +4211,15 @@
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="42.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.75" customWidth="1"/>
     <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -3997,7 +4233,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>291</v>
       </c>
@@ -4005,7 +4241,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>293</v>
       </c>
@@ -4013,7 +4249,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
@@ -4027,7 +4263,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>381</v>
       </c>
@@ -4035,7 +4271,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>285</v>
       </c>
@@ -4049,7 +4285,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>286</v>
       </c>
@@ -4063,7 +4299,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>303</v>
       </c>
@@ -4077,7 +4313,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>322</v>
       </c>
@@ -4091,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>305</v>
       </c>
@@ -4099,7 +4335,7 @@
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>306</v>
       </c>
@@ -4107,7 +4343,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>308</v>
       </c>
@@ -4115,7 +4351,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>310</v>
       </c>
@@ -4129,7 +4365,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="18" customFormat="1" ht="38" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -4143,7 +4379,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>311</v>
       </c>
@@ -4157,7 +4393,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="18" customFormat="1" ht="89" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>312</v>
       </c>
@@ -4168,7 +4404,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>414</v>
       </c>
@@ -4176,7 +4412,7 @@
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>415</v>
       </c>
@@ -4252,15 +4488,15 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.75" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.58203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -4274,7 +4510,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>283</v>
       </c>
@@ -4288,7 +4524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>284</v>
       </c>
@@ -4302,7 +4538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>11</v>
       </c>
@@ -4316,7 +4552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>376</v>
       </c>
@@ -4324,7 +4560,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>383</v>
       </c>
@@ -4335,7 +4571,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>384</v>
       </c>
@@ -4346,7 +4582,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="18" customFormat="1" ht="140" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>285</v>
       </c>
@@ -4360,7 +4596,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>286</v>
       </c>
@@ -4374,7 +4610,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>367</v>
       </c>
@@ -4383,7 +4619,7 @@
       </c>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>287</v>
       </c>
@@ -4489,17 +4725,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -4513,7 +4751,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>371</v>
       </c>
@@ -4523,7 +4761,7 @@
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>300</v>
       </c>
@@ -4537,7 +4775,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>296</v>
       </c>
@@ -4549,7 +4787,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="63.5" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>372</v>
       </c>
@@ -4591,21 +4829,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.58203125" customWidth="1"/>
+    <col min="2" max="2" width="27.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -4642,7 +4880,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4653,7 +4891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4699,13 +4937,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -4716,7 +4954,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -4727,7 +4965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4738,7 +4976,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -4749,7 +4987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -4760,7 +4998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
@@ -4771,7 +5009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>235</v>
       </c>
@@ -4782,7 +5020,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -4793,7 +5031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -4804,7 +5042,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -4815,7 +5053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -4826,7 +5064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -4837,7 +5075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -4848,7 +5086,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4859,7 +5097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>247</v>
       </c>
@@ -4870,7 +5108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>248</v>
       </c>
@@ -4881,7 +5119,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>249</v>
       </c>
@@ -4892,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>250</v>
       </c>
@@ -4903,7 +5141,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>251</v>
       </c>
@@ -4914,7 +5152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>252</v>
       </c>
@@ -4925,7 +5163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>253</v>
       </c>
@@ -4936,7 +5174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>254</v>
       </c>
@@ -4947,7 +5185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>255</v>
       </c>
@@ -4958,7 +5196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>256</v>
       </c>
@@ -4969,7 +5207,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>257</v>
       </c>
@@ -4980,7 +5218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>258</v>
       </c>
@@ -4991,7 +5229,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>259</v>
       </c>
@@ -5002,7 +5240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>260</v>
       </c>
@@ -5013,7 +5251,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>261</v>
       </c>
@@ -5024,7 +5262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>262</v>
       </c>
@@ -5035,7 +5273,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="11" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>263</v>
       </c>
@@ -5046,7 +5284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -5057,7 +5295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -5119,13 +5357,13 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -5136,67 +5374,67 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -5252,13 +5490,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -5269,112 +5507,112 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>263</v>
       </c>

</xml_diff>